<commit_message>
Worked on XLST and made some other changes too
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="22040" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="35580" yWindow="-3800" windowWidth="30480" windowHeight="20780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="187">
   <si>
     <t>Required?</t>
   </si>
@@ -581,6 +581,9 @@
   </si>
   <si>
     <t>gmd: language</t>
+  </si>
+  <si>
+    <t>connect to NKN datastore</t>
   </si>
 </sst>
 </file>
@@ -817,7 +820,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -870,17 +873,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="159">
@@ -1377,18 +1383,18 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="38.33203125" style="10" customWidth="1"/>
@@ -1410,14 +1416,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1494,16 +1500,16 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1521,7 +1527,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="19" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1538,10 +1544,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1557,7 +1563,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="18"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1575,10 +1581,10 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="21" t="s">
         <v>9</v>
       </c>
@@ -1600,7 +1606,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="19"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1612,10 +1618,10 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="21"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
@@ -1630,7 +1636,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="18"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1645,10 +1651,10 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="21"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
@@ -1663,7 +1669,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="18"/>
+      <c r="M7" s="19"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1672,12 +1678,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="19" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1692,7 +1698,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="18"/>
+      <c r="M8" s="19"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1707,12 +1713,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="18"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1725,7 +1731,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="18"/>
+      <c r="M9" s="19"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1740,12 +1746,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="18"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1758,7 +1764,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="18"/>
+      <c r="M10" s="19"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1770,12 +1776,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="18"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1788,7 +1794,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="18"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1806,12 +1812,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="18"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1824,7 +1830,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="18"/>
+      <c r="M12" s="19"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1836,12 +1842,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="21"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1854,7 +1860,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="18"/>
+      <c r="M13" s="19"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1872,12 +1878,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="18"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1890,7 +1896,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="18"/>
+      <c r="M14" s="19"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1905,12 +1911,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="18"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1923,7 +1929,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="18"/>
+      <c r="M15" s="19"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1935,9 +1941,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1956,7 +1962,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="18" t="s">
+      <c r="M16" s="19" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -1970,9 +1976,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1991,7 +1997,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="18"/>
+      <c r="M17" s="19"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2006,10 +2012,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="18" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2027,7 +2033,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="18"/>
+      <c r="M18" s="19"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2048,10 +2054,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2067,7 +2073,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="M19" s="19"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2088,13 +2094,13 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="75">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="M20" s="18"/>
+      <c r="M20" s="19"/>
       <c r="N20" s="2" t="s">
         <v>142</v>
       </c>
@@ -2118,14 +2124,14 @@
       </c>
     </row>
     <row r="21" spans="1:23" ht="90">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="18" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="2" t="s">
         <v>117</v>
       </c>
@@ -2141,7 +2147,7 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="18"/>
+      <c r="M21" s="19"/>
       <c r="N21" s="2" t="s">
         <v>57</v>
       </c>
@@ -2162,12 +2168,12 @@
       </c>
     </row>
     <row r="22" spans="1:23" ht="45">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="2" t="s">
         <v>116</v>
       </c>
@@ -2183,7 +2189,7 @@
       <c r="K22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="18"/>
+      <c r="M22" s="19"/>
       <c r="N22" s="2" t="s">
         <v>57</v>
       </c>
@@ -2207,14 +2213,14 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="90">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="18" t="s">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="19" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -2232,7 +2238,7 @@
       <c r="K23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M23" s="18" t="s">
+      <c r="M23" s="19" t="s">
         <v>108</v>
       </c>
       <c r="Q23" s="2" t="s">
@@ -2252,12 +2258,12 @@
       </c>
     </row>
     <row r="24" spans="1:23">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2270,7 +2276,7 @@
       <c r="K24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="18"/>
+      <c r="M24" s="19"/>
       <c r="S24" s="2">
         <v>-117.531786</v>
       </c>
@@ -2279,12 +2285,12 @@
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="2" t="s">
         <v>46</v>
       </c>
@@ -2297,7 +2303,7 @@
       <c r="K25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="18"/>
+      <c r="M25" s="19"/>
       <c r="S25" s="2">
         <v>-110.655421</v>
       </c>
@@ -2306,12 +2312,12 @@
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="2" t="s">
         <v>47</v>
       </c>
@@ -2324,7 +2330,7 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="18"/>
+      <c r="M26" s="19"/>
       <c r="S26" s="2">
         <v>41.946097000000002</v>
       </c>
@@ -2333,12 +2339,12 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
       <c r="G27" s="2" t="s">
         <v>48</v>
       </c>
@@ -2351,7 +2357,7 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="18"/>
+      <c r="M27" s="19"/>
       <c r="S27" s="2">
         <v>49.039541999999997</v>
       </c>
@@ -2360,12 +2366,12 @@
       </c>
     </row>
     <row r="28" spans="1:23" ht="30">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18" t="s">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19" t="s">
         <v>51</v>
       </c>
       <c r="G28" s="2" t="s">
@@ -2380,18 +2386,18 @@
       <c r="K28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M28" s="18"/>
+      <c r="M28" s="19"/>
       <c r="T28" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="2" t="s">
         <v>53</v>
       </c>
@@ -2404,18 +2410,18 @@
       <c r="K29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M29" s="18"/>
+      <c r="M29" s="19"/>
       <c r="T29" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="2" t="s">
         <v>54</v>
       </c>
@@ -2428,20 +2434,20 @@
       <c r="K30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="18"/>
+      <c r="M30" s="19"/>
       <c r="T30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="85" customHeight="1">
-      <c r="A31" s="19"/>
-      <c r="B31" s="18" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="19" t="s">
         <v>102</v>
       </c>
       <c r="E31" s="21" t="s">
@@ -2483,10 +2489,10 @@
       </c>
     </row>
     <row r="32" spans="1:23" ht="30" customHeight="1">
-      <c r="A32" s="19"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="21"/>
       <c r="F32" s="2"/>
       <c r="G32" s="10" t="s">
@@ -2501,7 +2507,7 @@
       <c r="K32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M32" s="18" t="s">
+      <c r="M32" s="19" t="s">
         <v>107</v>
       </c>
       <c r="N32" s="12" t="s">
@@ -2512,10 +2518,10 @@
       </c>
     </row>
     <row r="33" spans="1:23" ht="30">
-      <c r="A33" s="19"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="21"/>
       <c r="F33" s="7"/>
       <c r="G33" s="2" t="s">
@@ -2530,7 +2536,7 @@
       <c r="K33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M33" s="18"/>
+      <c r="M33" s="19"/>
       <c r="N33" s="2" t="s">
         <v>57</v>
       </c>
@@ -2542,12 +2548,12 @@
       </c>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="19"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="19" t="s">
         <v>16</v>
       </c>
       <c r="G34" s="2" t="s">
@@ -2559,7 +2565,7 @@
       <c r="K34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="18"/>
+      <c r="M34" s="19"/>
       <c r="N34" s="2" t="s">
         <v>77</v>
       </c>
@@ -2571,12 +2577,12 @@
       </c>
     </row>
     <row r="35" spans="1:23" ht="30">
-      <c r="A35" s="19"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="21"/>
-      <c r="F35" s="18"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="2" t="s">
         <v>16</v>
       </c>
@@ -2589,7 +2595,7 @@
       <c r="K35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="18"/>
+      <c r="M35" s="19"/>
       <c r="N35" s="2" t="s">
         <v>57</v>
       </c>
@@ -2601,12 +2607,12 @@
       </c>
     </row>
     <row r="36" spans="1:23" ht="30">
-      <c r="A36" s="19"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="20"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="21"/>
-      <c r="F36" s="18"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="2" t="s">
         <v>18</v>
       </c>
@@ -2619,7 +2625,7 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="18"/>
+      <c r="M36" s="19"/>
       <c r="N36" s="2" t="s">
         <v>57</v>
       </c>
@@ -2631,12 +2637,12 @@
       </c>
     </row>
     <row r="37" spans="1:23" ht="30">
-      <c r="A37" s="19"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="21"/>
-      <c r="F37" s="18"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="2" t="s">
         <v>19</v>
       </c>
@@ -2649,7 +2655,7 @@
       <c r="K37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="18"/>
+      <c r="M37" s="19"/>
       <c r="N37" s="2" t="s">
         <v>57</v>
       </c>
@@ -2661,12 +2667,12 @@
       </c>
     </row>
     <row r="38" spans="1:23" ht="30">
-      <c r="A38" s="19"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="21"/>
-      <c r="F38" s="18"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="2" t="s">
         <v>20</v>
       </c>
@@ -2679,7 +2685,7 @@
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="18"/>
+      <c r="M38" s="19"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
@@ -2691,12 +2697,12 @@
       </c>
     </row>
     <row r="39" spans="1:23" ht="30">
-      <c r="A39" s="19"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="21"/>
-      <c r="F39" s="18"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="2" t="s">
         <v>69</v>
       </c>
@@ -2709,7 +2715,7 @@
       <c r="K39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M39" s="18"/>
+      <c r="M39" s="19"/>
       <c r="N39" s="2" t="s">
         <v>57</v>
       </c>
@@ -2721,12 +2727,12 @@
       </c>
     </row>
     <row r="40" spans="1:23" ht="45">
-      <c r="A40" s="19"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="21"/>
-      <c r="F40" s="18"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="2" t="s">
         <v>15</v>
       </c>
@@ -2739,7 +2745,7 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="18"/>
+      <c r="M40" s="19"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
@@ -2754,12 +2760,12 @@
       </c>
     </row>
     <row r="41" spans="1:23" ht="30">
-      <c r="A41" s="19"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="21"/>
-      <c r="F41" s="18"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="2" t="s">
         <v>21</v>
       </c>
@@ -2772,7 +2778,7 @@
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="18"/>
+      <c r="M41" s="19"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
@@ -2784,11 +2790,12 @@
       </c>
     </row>
     <row r="42" spans="1:23" ht="90">
-      <c r="A42" s="19"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="G42" s="8" t="s">
+      <c r="A42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="21"/>
+      <c r="G42" s="22" t="s">
         <v>52</v>
       </c>
       <c r="H42" s="2" t="s">
@@ -2820,7 +2827,7 @@
       </c>
     </row>
     <row r="43" spans="1:23" ht="30">
-      <c r="A43" s="19"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="3" t="s">
         <v>94</v>
       </c>
@@ -2862,7 +2869,7 @@
       </c>
     </row>
     <row r="44" spans="1:23" ht="30">
-      <c r="A44" s="19"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="3" t="s">
         <v>149</v>
       </c>
@@ -3110,7 +3117,7 @@
         <v>172</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>6</v>
@@ -3200,16 +3207,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D23:D30"/>
-    <mergeCell ref="C3:C30"/>
     <mergeCell ref="M32:M41"/>
     <mergeCell ref="A3:A44"/>
     <mergeCell ref="B3:B30"/>
@@ -3221,10 +3218,20 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="M16:M22"/>
     <mergeCell ref="D31:D42"/>
-    <mergeCell ref="E31:E41"/>
     <mergeCell ref="F34:F41"/>
     <mergeCell ref="C31:C42"/>
     <mergeCell ref="B31:B42"/>
+    <mergeCell ref="E31:E42"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="D3:D15"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="E5:E15"/>
+    <mergeCell ref="D23:D30"/>
+    <mergeCell ref="C3:C30"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
Made changes to the Design Doc- added update frequency field; added guiding text and info for status field
XSLT- Complete for the fields that are currently in the editor. Parses
multiple contacts correctly. Fully commented for all parts, including
fields still to be added to mdedit form.
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35580" yWindow="-3800" windowWidth="30480" windowHeight="20780" tabRatio="500"/>
+    <workbookView xWindow="34240" yWindow="-2840" windowWidth="30480" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$45</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$G:$G,Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="193">
   <si>
     <t>Required?</t>
   </si>
@@ -584,6 +584,24 @@
   </si>
   <si>
     <t>connect to NKN datastore</t>
+  </si>
+  <si>
+    <t>What is the status of your dataset? For example, is it complete (you anticipate no further work and consider it final) or is it ongoing (continually being updated)?</t>
+  </si>
+  <si>
+    <t>Data Update Frequency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;gmd:MD_MaintenanceFrequencyCode </t>
+  </si>
+  <si>
+    <t>Drop-down list from ISO codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_MaintenanceFrequencyCode"</t>
+  </si>
+  <si>
+    <t>Value for List: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, asNeeded, irregular, noPlanned, unknown</t>
+  </si>
+  <si>
+    <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are availabel if you do not plan to update your data or do not know the specific frequency of updates.</t>
   </si>
 </sst>
 </file>
@@ -636,7 +654,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +664,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -820,7 +844,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -873,8 +897,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -885,8 +909,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="159">
@@ -1380,13 +1407,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1416,14 +1443,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2100,6 +2127,18 @@
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
+      <c r="H20" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="M20" s="19"/>
       <c r="N20" s="2" t="s">
         <v>142</v>
@@ -2123,23 +2162,18 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="90">
+    <row r="21" spans="1:23" ht="105">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>130</v>
+      <c r="G21" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>192</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>6</v>
@@ -2149,42 +2183,41 @@
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="2" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
       <c r="T21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="45">
+        <v>190</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="90">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
-      <c r="D22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>131</v>
+      </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>7</v>
@@ -2199,9 +2232,6 @@
       <c r="Q22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R22" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="S22" s="2" t="s">
         <v>118</v>
       </c>
@@ -2212,40 +2242,43 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="90">
+    <row r="23" spans="1:23" ht="45">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
-      <c r="D23" s="19" t="s">
-        <v>89</v>
-      </c>
+      <c r="D23" s="19"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="F23" s="19"/>
       <c r="G23" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M23" s="19" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="M23" s="19"/>
+      <c r="N23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="R23" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="S23" s="2" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="T23" s="2" t="s">
         <v>7</v>
@@ -2253,35 +2286,50 @@
       <c r="U23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="W23" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23">
+    </row>
+    <row r="24" spans="1:23" ht="90">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
-      <c r="D24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
+      <c r="F24" s="19" t="s">
+        <v>33</v>
+      </c>
       <c r="G24" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M24" s="19"/>
-      <c r="S24" s="2">
-        <v>-117.531786</v>
+        <v>11</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -2292,7 +2340,7 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>41</v>
@@ -2305,7 +2353,7 @@
       </c>
       <c r="M25" s="19"/>
       <c r="S25" s="2">
-        <v>-110.655421</v>
+        <v>-117.531786</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>11</v>
@@ -2319,7 +2367,7 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>41</v>
@@ -2332,7 +2380,7 @@
       </c>
       <c r="M26" s="19"/>
       <c r="S26" s="2">
-        <v>41.946097000000002</v>
+        <v>-110.655421</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>11</v>
@@ -2346,7 +2394,7 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>41</v>
@@ -2359,60 +2407,63 @@
       </c>
       <c r="M27" s="19"/>
       <c r="S27" s="2">
-        <v>49.039541999999997</v>
+        <v>41.946097000000002</v>
       </c>
       <c r="T27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="30">
+    <row r="28" spans="1:23">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="19" t="s">
-        <v>51</v>
-      </c>
+      <c r="F28" s="19"/>
       <c r="G28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>120</v>
+        <v>48</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M28" s="19"/>
+      <c r="S28" s="2">
+        <v>49.039541999999997</v>
+      </c>
       <c r="T28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="30">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="F29" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="G29" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M29" s="19"/>
       <c r="T29" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -2423,7 +2474,7 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>39</v>
@@ -2439,95 +2490,90 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="85" customHeight="1">
+    <row r="31" spans="1:23">
       <c r="A31" s="20"/>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M31" s="19"/>
+      <c r="T31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="85" customHeight="1">
+      <c r="A32" s="20"/>
+      <c r="B32" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C32" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D32" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E32" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="10" t="s">
+      <c r="F32" s="2"/>
+      <c r="G32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L31" s="2" t="s">
+      <c r="I32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="M32" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="R32" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="T32" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="U32" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="W31" s="2" t="s">
+      <c r="W32" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="30" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M32" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="T32" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" ht="30">
+    <row r="33" spans="1:21" ht="30" customHeight="1">
       <c r="A33" s="20"/>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
       <c r="E33" s="21"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="F33" s="2"/>
+      <c r="G33" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I33" s="10" t="s">
         <v>37</v>
       </c>
       <c r="J33" s="2" t="s">
@@ -2536,77 +2582,76 @@
       <c r="K33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M33" s="19"/>
-      <c r="N33" s="2" t="s">
+      <c r="M33" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N33" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="O33" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="T33" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:21" ht="30">
       <c r="A34" s="20"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="19" t="s">
-        <v>16</v>
-      </c>
+      <c r="F34" s="7"/>
       <c r="G34" s="2" t="s">
-        <v>73</v>
+        <v>126</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M34" s="19"/>
       <c r="N34" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="T34" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="30">
+    <row r="35" spans="1:21">
       <c r="A35" s="20"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
       <c r="E35" s="21"/>
-      <c r="F35" s="19"/>
+      <c r="F35" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="G35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M35" s="19"/>
       <c r="N35" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="T35" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="30">
+    <row r="36" spans="1:21" ht="30">
       <c r="A36" s="20"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
@@ -2614,7 +2659,7 @@
       <c r="E36" s="21"/>
       <c r="F36" s="19"/>
       <c r="G36" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>37</v>
@@ -2630,13 +2675,13 @@
         <v>57</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T36" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="30">
+    <row r="37" spans="1:21" ht="30">
       <c r="A37" s="20"/>
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
@@ -2644,10 +2689,10 @@
       <c r="E37" s="21"/>
       <c r="F37" s="19"/>
       <c r="G37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>6</v>
@@ -2660,13 +2705,13 @@
         <v>57</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="T37" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="30">
+    <row r="38" spans="1:21" ht="30">
       <c r="A38" s="20"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
@@ -2674,10 +2719,10 @@
       <c r="E38" s="21"/>
       <c r="F38" s="19"/>
       <c r="G38" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>6</v>
@@ -2690,13 +2735,13 @@
         <v>57</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T38" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="30">
+    <row r="39" spans="1:21" ht="30">
       <c r="A39" s="20"/>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -2704,10 +2749,10 @@
       <c r="E39" s="21"/>
       <c r="F39" s="19"/>
       <c r="G39" s="2" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>6</v>
@@ -2720,13 +2765,13 @@
         <v>57</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="T39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="45">
+    <row r="40" spans="1:21" ht="30">
       <c r="A40" s="20"/>
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
@@ -2734,13 +2779,13 @@
       <c r="E40" s="21"/>
       <c r="F40" s="19"/>
       <c r="G40" s="2" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>7</v>
@@ -2750,16 +2795,13 @@
         <v>57</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="T40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="30">
+    <row r="41" spans="1:21" ht="45">
       <c r="A41" s="20"/>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -2767,13 +2809,13 @@
       <c r="E41" s="21"/>
       <c r="F41" s="19"/>
       <c r="G41" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>7</v>
@@ -2783,136 +2825,133 @@
         <v>57</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="T41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="90">
+    <row r="42" spans="1:21" ht="30">
       <c r="A42" s="20"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="21"/>
-      <c r="G42" s="22" t="s">
+      <c r="F42" s="19"/>
+      <c r="G42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="19"/>
+      <c r="N42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="90">
+      <c r="A43" s="20"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="21"/>
+      <c r="G43" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M42" s="4" t="s">
+      <c r="J43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="N42" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O42" s="2" t="s">
+      <c r="O43" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="P42" s="7" t="s">
+      <c r="P43" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="T42" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" ht="30">
-      <c r="A43" s="20"/>
-      <c r="B43" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H43" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M43" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N43" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R43" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="T43" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U43" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" ht="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="30">
       <c r="A44" s="20"/>
       <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="15"/>
+      <c r="G44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U44" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="30">
+      <c r="A45" s="20"/>
+      <c r="B45" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="E45" s="15"/>
+      <c r="G45" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="T44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23">
-      <c r="B45" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="H45" s="14" t="s">
         <v>151</v>
@@ -2926,31 +2965,31 @@
       <c r="M45" s="4" t="s">
         <v>152</v>
       </c>
+      <c r="N45" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="O45" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R45" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="T45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
       <c r="B46" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H46" s="14" t="s">
         <v>151</v>
@@ -2965,16 +3004,16 @@
         <v>152</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>185</v>
+        <v>156</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="T46" s="2" t="s">
         <v>7</v>
@@ -2983,12 +3022,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:21">
       <c r="B47" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H47" s="14" t="s">
         <v>151</v>
@@ -3003,16 +3042,16 @@
         <v>152</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>161</v>
+        <v>28</v>
       </c>
       <c r="T47" s="2" t="s">
         <v>7</v>
@@ -3021,12 +3060,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="45">
+    <row r="48" spans="1:21">
       <c r="B48" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H48" s="14" t="s">
         <v>151</v>
@@ -3040,20 +3079,17 @@
       <c r="M48" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="N48" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="O48" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="T48" s="2" t="s">
         <v>7</v>
@@ -3061,16 +3097,13 @@
       <c r="U48" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="W48" s="2" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="49" spans="2:23" ht="45">
       <c r="B49" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H49" s="14" t="s">
         <v>151</v>
@@ -3088,16 +3121,16 @@
         <v>57</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R49" s="2">
-        <v>2003</v>
+      <c r="R49" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="T49" s="2" t="s">
         <v>7</v>
@@ -3109,15 +3142,15 @@
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="2:23" ht="30">
+    <row r="50" spans="2:23" ht="45">
       <c r="B50" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>6</v>
@@ -3132,30 +3165,36 @@
         <v>57</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="R50" s="2">
+        <v>2003</v>
+      </c>
       <c r="T50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23">
+        <v>162</v>
+      </c>
+      <c r="W50" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" ht="30">
       <c r="B51" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>6</v>
@@ -3166,22 +3205,31 @@
       <c r="M51" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="R51" s="2" t="s">
-        <v>178</v>
+      <c r="N51" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="T51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="2:23" ht="75">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23">
       <c r="B52" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>151</v>
@@ -3196,7 +3244,7 @@
         <v>152</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T52" s="2" t="s">
         <v>7</v>
@@ -3205,41 +3253,70 @@
         <v>162</v>
       </c>
     </row>
+    <row r="53" spans="2:23" ht="75">
+      <c r="B53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U53" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="M32:M41"/>
-    <mergeCell ref="A3:A44"/>
-    <mergeCell ref="B3:B30"/>
-    <mergeCell ref="M3:M15"/>
-    <mergeCell ref="M23:M30"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M16:M22"/>
-    <mergeCell ref="D31:D42"/>
-    <mergeCell ref="F34:F41"/>
-    <mergeCell ref="C31:C42"/>
-    <mergeCell ref="B31:B42"/>
-    <mergeCell ref="E31:E42"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="E29:E31"/>
     <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="F24:F28"/>
     <mergeCell ref="F8:F15"/>
     <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D23:D30"/>
-    <mergeCell ref="C3:C30"/>
+    <mergeCell ref="D24:D31"/>
+    <mergeCell ref="C3:C31"/>
+    <mergeCell ref="M33:M42"/>
+    <mergeCell ref="A3:A45"/>
+    <mergeCell ref="B3:B31"/>
+    <mergeCell ref="M3:M15"/>
+    <mergeCell ref="M24:M31"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="M16:M23"/>
+    <mergeCell ref="D32:D43"/>
+    <mergeCell ref="F35:F42"/>
+    <mergeCell ref="C32:C43"/>
+    <mergeCell ref="B32:B43"/>
+    <mergeCell ref="E32:E43"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="21" fitToHeight="2" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="27" max="16383" man="1"/>
-    <brk id="43" max="16383" man="1"/>
+    <brk id="28" max="16383" man="1"/>
+    <brk id="44" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>

</xml_diff>

<commit_message>
updated status field dropdown values if statement in xslt
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34240" yWindow="-2840" windowWidth="30480" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="-400" yWindow="280" windowWidth="30480" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,9 +448,6 @@
     <t>Drop-down list from ISO Progress Codes.  codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_ProgressCode</t>
   </si>
   <si>
-    <t>Values for List: completed, continually updated, in progress, planned. ISO values for xml: completed, historicalArchive, obsolete, onGoing, planned, required, underDevelopment</t>
-  </si>
-  <si>
     <t>gmd:MD_ProgressCode_PropertyType</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are availabel if you do not plan to update your data or do not know the specific frequency of updates.</t>
+  </si>
+  <si>
+    <t>Values for List: completed, continually updated, in process, planned, needs to be generated or updated, stored in an offline facility, no longer valid. ISO values for xml: completed, onGoing, underDevelopment, planned, required, historicalArchive, obsolete</t>
   </si>
 </sst>
 </file>
@@ -900,6 +900,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -908,12 +914,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="159">
@@ -1410,10 +1410,10 @@
   <dimension ref="A1:W53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1443,14 +1443,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1511,14 +1511,14 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>181</v>
-      </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1527,16 +1527,16 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="22" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1554,7 +1554,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M3" s="21" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1571,10 +1571,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="19"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1608,11 +1608,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1633,7 +1633,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="19"/>
+      <c r="M5" s="21"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1645,11 +1645,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1663,7 +1663,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="19"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1678,11 +1678,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1696,7 +1696,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="19"/>
+      <c r="M7" s="21"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1705,12 +1705,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="19" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1725,7 +1725,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="19"/>
+      <c r="M8" s="21"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1740,12 +1740,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="19"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1758,7 +1758,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="19"/>
+      <c r="M9" s="21"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1773,12 +1773,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="19"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1791,7 +1791,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="19"/>
+      <c r="M10" s="21"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1803,12 +1803,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="19"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="19"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1839,12 +1839,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1857,7 +1857,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="19"/>
+      <c r="M12" s="21"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1869,12 +1869,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="19"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="19"/>
+      <c r="M13" s="21"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1905,12 +1905,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="19"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="19"/>
+      <c r="M14" s="21"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1938,12 +1938,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1956,7 +1956,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="19"/>
+      <c r="M15" s="21"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1968,9 +1968,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="19" t="s">
+      <c r="M16" s="21" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2003,9 +2003,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="19"/>
+      <c r="M17" s="21"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2039,17 +2039,17 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="19" t="s">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>135</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>40</v>
@@ -2060,7 +2060,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="19"/>
+      <c r="M18" s="21"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2081,10 +2081,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="19"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="19"/>
+      <c r="M19" s="21"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>98</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T19" s="2" t="s">
         <v>6</v>
@@ -2120,15 +2120,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="75">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
+    <row r="20" spans="1:23" ht="90">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>38</v>
@@ -2139,9 +2139,9 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="19"/>
+      <c r="M20" s="21"/>
       <c r="N20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>138</v>
@@ -2159,18 +2159,18 @@
         <v>140</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="105">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="G21" s="23" t="s">
-        <v>188</v>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="G21" s="19" t="s">
+        <v>187</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>38</v>
@@ -2181,32 +2181,32 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="19"/>
+      <c r="M21" s="21"/>
       <c r="N21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U21" s="2" t="s">
+      <c r="V21" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="V21" s="2" t="s">
-        <v>191</v>
-      </c>
     </row>
     <row r="22" spans="1:23" ht="90">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="19" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="2" t="s">
         <v>117</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="K22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="19"/>
+      <c r="M22" s="21"/>
       <c r="N22" s="2" t="s">
         <v>57</v>
       </c>
@@ -2243,12 +2243,12 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="45">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="2" t="s">
         <v>116</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="19"/>
+      <c r="M23" s="21"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>72</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>118</v>
@@ -2288,21 +2288,21 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="90">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="19" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="s">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>44</v>
@@ -2313,7 +2313,7 @@
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="21" t="s">
         <v>108</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -2333,12 +2333,12 @@
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="2" t="s">
         <v>45</v>
       </c>
@@ -2351,7 +2351,7 @@
       <c r="K25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="19"/>
+      <c r="M25" s="21"/>
       <c r="S25" s="2">
         <v>-117.531786</v>
       </c>
@@ -2360,12 +2360,12 @@
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="19"/>
+      <c r="M26" s="21"/>
       <c r="S26" s="2">
         <v>-110.655421</v>
       </c>
@@ -2387,12 +2387,12 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="2" t="s">
         <v>47</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="19"/>
+      <c r="M27" s="21"/>
       <c r="S27" s="2">
         <v>41.946097000000002</v>
       </c>
@@ -2414,12 +2414,12 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="2" t="s">
         <v>48</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="19"/>
+      <c r="M28" s="21"/>
       <c r="S28" s="2">
         <v>49.039541999999997</v>
       </c>
@@ -2441,12 +2441,12 @@
       </c>
     </row>
     <row r="29" spans="1:23" ht="30">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21" t="s">
         <v>51</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2461,18 +2461,18 @@
       <c r="K29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="19"/>
+      <c r="M29" s="21"/>
       <c r="T29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="2" t="s">
         <v>53</v>
       </c>
@@ -2485,18 +2485,18 @@
       <c r="K30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="19"/>
+      <c r="M30" s="21"/>
       <c r="T30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="2" t="s">
         <v>54</v>
       </c>
@@ -2509,23 +2509,23 @@
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="19"/>
+      <c r="M31" s="21"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="85" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="19" t="s">
+      <c r="A32" s="22"/>
+      <c r="B32" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="23" t="s">
         <v>101</v>
       </c>
       <c r="F32" s="2"/>
@@ -2533,7 +2533,7 @@
         <v>11</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>11</v>
@@ -2545,30 +2545,30 @@
         <v>11</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>109</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="T32" s="2" t="s">
         <v>127</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="W32" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="30" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="21"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="2"/>
       <c r="G33" s="10" t="s">
         <v>124</v>
@@ -2582,7 +2582,7 @@
       <c r="K33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M33" s="19" t="s">
+      <c r="M33" s="21" t="s">
         <v>107</v>
       </c>
       <c r="N33" s="12" t="s">
@@ -2593,11 +2593,11 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="30">
-      <c r="A34" s="20"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="21"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="7"/>
       <c r="G34" s="2" t="s">
         <v>126</v>
@@ -2611,7 +2611,7 @@
       <c r="K34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="19"/>
+      <c r="M34" s="21"/>
       <c r="N34" s="2" t="s">
         <v>57</v>
       </c>
@@ -2623,12 +2623,12 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="20"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="19" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -2640,7 +2640,7 @@
       <c r="K35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="19"/>
+      <c r="M35" s="21"/>
       <c r="N35" s="2" t="s">
         <v>77</v>
       </c>
@@ -2652,12 +2652,12 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="30">
-      <c r="A36" s="20"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="19"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="2" t="s">
         <v>16</v>
       </c>
@@ -2670,7 +2670,7 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="19"/>
+      <c r="M36" s="21"/>
       <c r="N36" s="2" t="s">
         <v>57</v>
       </c>
@@ -2682,12 +2682,12 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="30">
-      <c r="A37" s="20"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="19"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="2" t="s">
         <v>18</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="K37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="19"/>
+      <c r="M37" s="21"/>
       <c r="N37" s="2" t="s">
         <v>57</v>
       </c>
@@ -2712,12 +2712,12 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="30">
-      <c r="A38" s="20"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="19"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="21"/>
       <c r="G38" s="2" t="s">
         <v>19</v>
       </c>
@@ -2730,7 +2730,7 @@
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="19"/>
+      <c r="M38" s="21"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
@@ -2742,12 +2742,12 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="30">
-      <c r="A39" s="20"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="19"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="2" t="s">
         <v>20</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="K39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M39" s="19"/>
+      <c r="M39" s="21"/>
       <c r="N39" s="2" t="s">
         <v>57</v>
       </c>
@@ -2772,12 +2772,12 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="30">
-      <c r="A40" s="20"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="19"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="21"/>
       <c r="G40" s="2" t="s">
         <v>69</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="19"/>
+      <c r="M40" s="21"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
@@ -2802,12 +2802,12 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="45">
-      <c r="A41" s="20"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="19"/>
+      <c r="A41" s="22"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="21"/>
       <c r="G41" s="2" t="s">
         <v>15</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="19"/>
+      <c r="M41" s="21"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
@@ -2835,12 +2835,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="30">
-      <c r="A42" s="20"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="19"/>
+      <c r="A42" s="22"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="21"/>
       <c r="G42" s="2" t="s">
         <v>21</v>
       </c>
@@ -2853,7 +2853,7 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="19"/>
+      <c r="M42" s="21"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
@@ -2865,19 +2865,19 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="90">
-      <c r="A43" s="20"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="21"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="23"/>
       <c r="G43" s="18" t="s">
         <v>52</v>
       </c>
       <c r="H43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>7</v>
@@ -2902,7 +2902,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="30">
-      <c r="A44" s="20"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="3" t="s">
         <v>94</v>
       </c>
@@ -2945,34 +2945,34 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="30">
-      <c r="A45" s="20"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="15"/>
       <c r="G45" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H45" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="J45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M45" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M45" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>6</v>
@@ -2981,71 +2981,71 @@
         <v>7</v>
       </c>
       <c r="U45" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:21">
       <c r="B46" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O46" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="O46" s="2" t="s">
+      <c r="P46" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R46" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="P46" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="T46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U46" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:21">
       <c r="B47" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H47" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="J47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="O47" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>6</v>
@@ -3057,118 +3057,118 @@
         <v>7</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:21">
       <c r="B48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R48" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R48" s="2" t="s">
+      <c r="T48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U48" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="T48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U48" s="2" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="49" spans="2:23" ht="45">
       <c r="B49" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H49" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M49" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M49" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R49" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U49" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W49" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="T49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U49" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="W49" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="50" spans="2:23" ht="45">
       <c r="B50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H50" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M50" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>6</v>
@@ -3180,21 +3180,21 @@
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="2:23" ht="30">
       <c r="B51" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="H51" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>6</v>
@@ -3203,16 +3203,16 @@
         <v>7</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>6</v>
@@ -3221,79 +3221,69 @@
         <v>7</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="2:23">
       <c r="B52" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H52" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M52" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M52" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R52" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U52" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="2:23" ht="75">
       <c r="B53" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H53" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="J53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R53" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T53" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U53" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="C3:C31"/>
     <mergeCell ref="M33:M42"/>
     <mergeCell ref="A3:A45"/>
     <mergeCell ref="B3:B31"/>
@@ -3309,6 +3299,16 @@
     <mergeCell ref="C32:C43"/>
     <mergeCell ref="B32:B43"/>
     <mergeCell ref="E32:E43"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="D3:D15"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="E5:E15"/>
+    <mergeCell ref="D24:D31"/>
+    <mergeCell ref="C3:C31"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
edits to both for update frequency
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-400" yWindow="280" windowWidth="30480" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -595,13 +595,13 @@
     <t>Drop-down list from ISO codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_MaintenanceFrequencyCode"</t>
   </si>
   <si>
-    <t>Value for List: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, asNeeded, irregular, noPlanned, unknown</t>
-  </si>
-  <si>
     <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are availabel if you do not plan to update your data or do not know the specific frequency of updates.</t>
   </si>
   <si>
     <t>Values for List: completed, continually updated, in process, planned, needs to be generated or updated, stored in an offline facility, no longer valid. ISO values for xml: completed, onGoing, underDevelopment, planned, required, historicalArchive, obsolete</t>
+  </si>
+  <si>
+    <t>Value for List: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, as needed, irregular, not planned, unknown   For ISO: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, asNeeded, irregular, notPlanned, unknown</t>
   </si>
 </sst>
 </file>
@@ -903,9 +903,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -913,6 +910,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1410,10 +1410,10 @@
   <dimension ref="A1:W53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="V19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1443,14 +1443,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1527,16 +1527,16 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1554,7 +1554,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1571,10 +1571,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="20"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1608,11 +1608,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1633,7 +1633,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1645,11 +1645,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1663,7 +1663,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="21"/>
+      <c r="M6" s="20"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1678,11 +1678,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1696,7 +1696,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="21"/>
+      <c r="M7" s="20"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1705,12 +1705,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1725,7 +1725,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1740,12 +1740,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="21"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1758,7 +1758,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1773,12 +1773,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1791,7 +1791,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="21"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1803,12 +1803,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="21"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1839,12 +1839,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1857,7 +1857,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="21"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1869,12 +1869,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="21"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1905,12 +1905,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1923,7 +1923,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="21"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1938,12 +1938,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1956,7 +1956,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="21"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1968,9 +1968,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1989,7 +1989,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="20" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2003,9 +2003,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="21"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2039,10 +2039,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="20" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2060,7 +2060,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="21"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2081,10 +2081,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="21"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2121,9 +2121,9 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
@@ -2139,7 +2139,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="21"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2159,18 +2159,18 @@
         <v>140</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="105">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
       <c r="G21" s="19" t="s">
         <v>187</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>38</v>
@@ -2181,7 +2181,7 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="21"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="2" t="s">
         <v>188</v>
       </c>
@@ -2195,18 +2195,18 @@
         <v>189</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="90">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="2" t="s">
         <v>117</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="K22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="21"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="2" t="s">
         <v>57</v>
       </c>
@@ -2243,12 +2243,12 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="45">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="2" t="s">
         <v>116</v>
       </c>
@@ -2264,7 +2264,7 @@
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="21"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2288,14 +2288,14 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="90">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="21" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2313,7 +2313,7 @@
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="21" t="s">
+      <c r="M24" s="20" t="s">
         <v>108</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -2333,12 +2333,12 @@
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="2" t="s">
         <v>45</v>
       </c>
@@ -2351,7 +2351,7 @@
       <c r="K25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="21"/>
+      <c r="M25" s="20"/>
       <c r="S25" s="2">
         <v>-117.531786</v>
       </c>
@@ -2360,12 +2360,12 @@
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="21"/>
+      <c r="M26" s="20"/>
       <c r="S26" s="2">
         <v>-110.655421</v>
       </c>
@@ -2387,12 +2387,12 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="2" t="s">
         <v>47</v>
       </c>
@@ -2405,7 +2405,7 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="21"/>
+      <c r="M27" s="20"/>
       <c r="S27" s="2">
         <v>41.946097000000002</v>
       </c>
@@ -2414,12 +2414,12 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="2" t="s">
         <v>48</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="21"/>
+      <c r="M28" s="20"/>
       <c r="S28" s="2">
         <v>49.039541999999997</v>
       </c>
@@ -2441,12 +2441,12 @@
       </c>
     </row>
     <row r="29" spans="1:23" ht="30">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20" t="s">
         <v>51</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2461,18 +2461,18 @@
       <c r="K29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="21"/>
+      <c r="M29" s="20"/>
       <c r="T29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="2" t="s">
         <v>53</v>
       </c>
@@ -2485,18 +2485,18 @@
       <c r="K30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="21"/>
+      <c r="M30" s="20"/>
       <c r="T30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="2" t="s">
         <v>54</v>
       </c>
@@ -2509,23 +2509,23 @@
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="21"/>
+      <c r="M31" s="20"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="85" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="22" t="s">
         <v>101</v>
       </c>
       <c r="F32" s="2"/>
@@ -2564,11 +2564,11 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="30" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="23"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="2"/>
       <c r="G33" s="10" t="s">
         <v>124</v>
@@ -2582,7 +2582,7 @@
       <c r="K33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M33" s="21" t="s">
+      <c r="M33" s="20" t="s">
         <v>107</v>
       </c>
       <c r="N33" s="12" t="s">
@@ -2593,11 +2593,11 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="30">
-      <c r="A34" s="22"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="23"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="7"/>
       <c r="G34" s="2" t="s">
         <v>126</v>
@@ -2611,7 +2611,7 @@
       <c r="K34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="21"/>
+      <c r="M34" s="20"/>
       <c r="N34" s="2" t="s">
         <v>57</v>
       </c>
@@ -2623,12 +2623,12 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="22"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="21" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="20" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -2640,7 +2640,7 @@
       <c r="K35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="21"/>
+      <c r="M35" s="20"/>
       <c r="N35" s="2" t="s">
         <v>77</v>
       </c>
@@ -2652,12 +2652,12 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="30">
-      <c r="A36" s="22"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="21"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="2" t="s">
         <v>16</v>
       </c>
@@ -2670,7 +2670,7 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="21"/>
+      <c r="M36" s="20"/>
       <c r="N36" s="2" t="s">
         <v>57</v>
       </c>
@@ -2682,12 +2682,12 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="30">
-      <c r="A37" s="22"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="2" t="s">
         <v>18</v>
       </c>
@@ -2700,7 +2700,7 @@
       <c r="K37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="21"/>
+      <c r="M37" s="20"/>
       <c r="N37" s="2" t="s">
         <v>57</v>
       </c>
@@ -2712,12 +2712,12 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="30">
-      <c r="A38" s="22"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="21"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="2" t="s">
         <v>19</v>
       </c>
@@ -2730,7 +2730,7 @@
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="21"/>
+      <c r="M38" s="20"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
@@ -2742,12 +2742,12 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="30">
-      <c r="A39" s="22"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="21"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="2" t="s">
         <v>20</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="K39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M39" s="21"/>
+      <c r="M39" s="20"/>
       <c r="N39" s="2" t="s">
         <v>57</v>
       </c>
@@ -2772,12 +2772,12 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="30">
-      <c r="A40" s="22"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="21"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="2" t="s">
         <v>69</v>
       </c>
@@ -2790,7 +2790,7 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="21"/>
+      <c r="M40" s="20"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
@@ -2802,12 +2802,12 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="45">
-      <c r="A41" s="22"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="2" t="s">
         <v>15</v>
       </c>
@@ -2820,7 +2820,7 @@
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="21"/>
+      <c r="M41" s="20"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
@@ -2835,12 +2835,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="30">
-      <c r="A42" s="22"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="2" t="s">
         <v>21</v>
       </c>
@@ -2853,7 +2853,7 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="21"/>
+      <c r="M42" s="20"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
@@ -2865,11 +2865,11 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="90">
-      <c r="A43" s="22"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="23"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="22"/>
       <c r="G43" s="18" t="s">
         <v>52</v>
       </c>
@@ -2902,7 +2902,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="30">
-      <c r="A44" s="22"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="3" t="s">
         <v>94</v>
       </c>
@@ -2945,7 +2945,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="30">
-      <c r="A45" s="22"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="3" t="s">
         <v>148</v>
       </c>
@@ -3284,6 +3284,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="D3:D15"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="E5:E15"/>
+    <mergeCell ref="D24:D31"/>
+    <mergeCell ref="C3:C31"/>
     <mergeCell ref="M33:M42"/>
     <mergeCell ref="A3:A45"/>
     <mergeCell ref="B3:B31"/>
@@ -3299,16 +3309,6 @@
     <mergeCell ref="C32:C43"/>
     <mergeCell ref="B32:B43"/>
     <mergeCell ref="E32:E43"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="C3:C31"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
updates to xslt and design doc
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27460" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="190">
   <si>
     <t>Required?</t>
   </si>
@@ -587,6 +587,12 @@
   </si>
   <si>
     <t>Value for List: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, as needed, irregular, not planned, unknown   For ISO: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, asNeeded, irregular, notPlanned, unknown</t>
+  </si>
+  <si>
+    <t>Dropdown list</t>
+  </si>
+  <si>
+    <t>Values for List: dataset, series     ISO Values for xml: [same]</t>
   </si>
 </sst>
 </file>
@@ -668,8 +674,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -890,9 +904,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -902,8 +913,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -984,6 +998,10 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1064,6 +1082,10 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1399,10 +1421,10 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="T20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J30" sqref="J30:J31"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1432,14 +1454,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1514,18 +1536,24 @@
       <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="U2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1543,7 +1571,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1560,10 +1588,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1579,7 +1607,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="20"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1597,11 +1625,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1622,7 +1650,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1634,11 +1662,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1652,7 +1680,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="21"/>
+      <c r="M6" s="20"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1667,11 +1695,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1685,7 +1713,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="21"/>
+      <c r="M7" s="20"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1694,12 +1722,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1714,7 +1742,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1729,12 +1757,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="21"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1747,7 +1775,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="20"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1762,12 +1790,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1780,7 +1808,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="21"/>
+      <c r="M10" s="20"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1792,12 +1820,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1810,7 +1838,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="21"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1828,12 +1856,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1846,7 +1874,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="21"/>
+      <c r="M12" s="20"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1858,12 +1886,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1876,7 +1904,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="21"/>
+      <c r="M13" s="20"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1894,12 +1922,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1912,7 +1940,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="21"/>
+      <c r="M14" s="20"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1927,12 +1955,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1945,7 +1973,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="21"/>
+      <c r="M15" s="20"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1957,9 +1985,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1978,7 +2006,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="20" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -1992,9 +2020,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2013,7 +2041,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="21"/>
+      <c r="M17" s="20"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2028,10 +2056,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="20" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2049,7 +2077,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="21"/>
+      <c r="M18" s="20"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2070,10 +2098,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2089,7 +2117,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="21"/>
+      <c r="M19" s="20"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2110,9 +2138,9 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
@@ -2128,7 +2156,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="21"/>
+      <c r="M20" s="20"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2152,9 +2180,9 @@
       </c>
     </row>
     <row r="21" spans="1:23" ht="105">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
       <c r="G21" s="19" t="s">
         <v>182</v>
       </c>
@@ -2170,7 +2198,7 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="21"/>
+      <c r="M21" s="20"/>
       <c r="N21" s="2" t="s">
         <v>183</v>
       </c>
@@ -2188,14 +2216,14 @@
       </c>
     </row>
     <row r="22" spans="1:23" ht="90">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21" t="s">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="2" t="s">
         <v>117</v>
       </c>
@@ -2211,7 +2239,7 @@
       <c r="K22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="21"/>
+      <c r="M22" s="20"/>
       <c r="N22" s="2" t="s">
         <v>57</v>
       </c>
@@ -2232,12 +2260,12 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="45">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="2" t="s">
         <v>116</v>
       </c>
@@ -2253,7 +2281,7 @@
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="21"/>
+      <c r="M23" s="20"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2277,14 +2305,14 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="90">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="21" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2302,7 +2330,7 @@
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="21" t="s">
+      <c r="M24" s="20" t="s">
         <v>108</v>
       </c>
       <c r="Q24" s="2" t="s">
@@ -2322,12 +2350,12 @@
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="2" t="s">
         <v>45</v>
       </c>
@@ -2340,7 +2368,7 @@
       <c r="K25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M25" s="21"/>
+      <c r="M25" s="20"/>
       <c r="S25" s="2">
         <v>-117.531786</v>
       </c>
@@ -2349,12 +2377,12 @@
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="2" t="s">
         <v>46</v>
       </c>
@@ -2367,7 +2395,7 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="21"/>
+      <c r="M26" s="20"/>
       <c r="S26" s="2">
         <v>-110.655421</v>
       </c>
@@ -2376,12 +2404,12 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="2" t="s">
         <v>47</v>
       </c>
@@ -2394,7 +2422,7 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="21"/>
+      <c r="M27" s="20"/>
       <c r="S27" s="2">
         <v>41.946097000000002</v>
       </c>
@@ -2403,12 +2431,12 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="2" t="s">
         <v>48</v>
       </c>
@@ -2421,7 +2449,7 @@
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="21"/>
+      <c r="M28" s="20"/>
       <c r="S28" s="2">
         <v>49.039541999999997</v>
       </c>
@@ -2430,12 +2458,12 @@
       </c>
     </row>
     <row r="29" spans="1:23" ht="30">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20" t="s">
         <v>51</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -2450,18 +2478,18 @@
       <c r="K29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M29" s="21"/>
+      <c r="M29" s="20"/>
       <c r="T29" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="2" t="s">
         <v>53</v>
       </c>
@@ -2474,18 +2502,18 @@
       <c r="K30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="21"/>
+      <c r="M30" s="20"/>
       <c r="T30" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="2" t="s">
         <v>54</v>
       </c>
@@ -2498,23 +2526,23 @@
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="21"/>
+      <c r="M31" s="20"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="85" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="22" t="s">
         <v>101</v>
       </c>
       <c r="F32" s="2"/>
@@ -2553,11 +2581,11 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="30" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="23"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="2"/>
       <c r="G33" s="10" t="s">
         <v>124</v>
@@ -2571,7 +2599,7 @@
       <c r="K33" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M33" s="21" t="s">
+      <c r="M33" s="20" t="s">
         <v>107</v>
       </c>
       <c r="N33" s="12" t="s">
@@ -2582,11 +2610,11 @@
       </c>
     </row>
     <row r="34" spans="1:21" ht="30">
-      <c r="A34" s="22"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="23"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="7"/>
       <c r="G34" s="2" t="s">
         <v>126</v>
@@ -2600,7 +2628,7 @@
       <c r="K34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="21"/>
+      <c r="M34" s="20"/>
       <c r="N34" s="2" t="s">
         <v>57</v>
       </c>
@@ -2612,12 +2640,12 @@
       </c>
     </row>
     <row r="35" spans="1:21">
-      <c r="A35" s="22"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="21" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="20" t="s">
         <v>16</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -2629,7 +2657,7 @@
       <c r="K35" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M35" s="21"/>
+      <c r="M35" s="20"/>
       <c r="N35" s="2" t="s">
         <v>77</v>
       </c>
@@ -2641,12 +2669,12 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="30">
-      <c r="A36" s="22"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="21"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="20"/>
       <c r="G36" s="2" t="s">
         <v>16</v>
       </c>
@@ -2659,7 +2687,7 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M36" s="21"/>
+      <c r="M36" s="20"/>
       <c r="N36" s="2" t="s">
         <v>57</v>
       </c>
@@ -2671,12 +2699,12 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="30">
-      <c r="A37" s="22"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="20"/>
       <c r="G37" s="2" t="s">
         <v>18</v>
       </c>
@@ -2689,7 +2717,7 @@
       <c r="K37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="21"/>
+      <c r="M37" s="20"/>
       <c r="N37" s="2" t="s">
         <v>57</v>
       </c>
@@ -2701,12 +2729,12 @@
       </c>
     </row>
     <row r="38" spans="1:21" ht="30">
-      <c r="A38" s="22"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="21"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="20"/>
       <c r="G38" s="2" t="s">
         <v>19</v>
       </c>
@@ -2719,7 +2747,7 @@
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="21"/>
+      <c r="M38" s="20"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
@@ -2731,12 +2759,12 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="30">
-      <c r="A39" s="22"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="21"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="2" t="s">
         <v>20</v>
       </c>
@@ -2749,7 +2777,7 @@
       <c r="K39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M39" s="21"/>
+      <c r="M39" s="20"/>
       <c r="N39" s="2" t="s">
         <v>57</v>
       </c>
@@ -2761,12 +2789,12 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="30">
-      <c r="A40" s="22"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="21"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
       <c r="G40" s="2" t="s">
         <v>69</v>
       </c>
@@ -2779,7 +2807,7 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="21"/>
+      <c r="M40" s="20"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
@@ -2791,12 +2819,12 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="45">
-      <c r="A41" s="22"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="2" t="s">
         <v>15</v>
       </c>
@@ -2809,7 +2837,7 @@
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="21"/>
+      <c r="M41" s="20"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
@@ -2824,12 +2852,12 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="30">
-      <c r="A42" s="22"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="20"/>
       <c r="G42" s="2" t="s">
         <v>21</v>
       </c>
@@ -2842,7 +2870,7 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="21"/>
+      <c r="M42" s="20"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
@@ -2854,11 +2882,11 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="90">
-      <c r="A43" s="22"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="23"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="22"/>
       <c r="G43" s="18" t="s">
         <v>52</v>
       </c>
@@ -2891,7 +2919,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="30">
-      <c r="A44" s="22"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="3" t="s">
         <v>94</v>
       </c>
@@ -2934,7 +2962,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="30">
-      <c r="A45" s="22"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="3" t="s">
         <v>148</v>
       </c>
@@ -3235,6 +3263,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="D3:D15"/>
+    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="E5:E15"/>
+    <mergeCell ref="D24:D31"/>
+    <mergeCell ref="C3:C31"/>
     <mergeCell ref="M33:M42"/>
     <mergeCell ref="A3:A45"/>
     <mergeCell ref="B3:B31"/>
@@ -3250,16 +3288,6 @@
     <mergeCell ref="C32:C43"/>
     <mergeCell ref="B32:B43"/>
     <mergeCell ref="E32:E43"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F24:F28"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="C3:C31"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
updates with new fields
refer to the Fields Wiki page too
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27460" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="33580" yWindow="-3980" windowWidth="30980" windowHeight="20200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$50</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$G:$G,Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="206">
   <si>
     <t>Required?</t>
   </si>
@@ -593,6 +593,54 @@
   </si>
   <si>
     <t>Values for List: dataset, series     ISO Values for xml: [same]</t>
+  </si>
+  <si>
+    <t>Needs to be editable; even if NKN is choosen as distributor</t>
+  </si>
+  <si>
+    <t>Vertical Extent</t>
+  </si>
+  <si>
+    <t>Vertical Minimum</t>
+  </si>
+  <si>
+    <t>Vertical Maximum</t>
+  </si>
+  <si>
+    <t>What is the minimum and maximum vertical heights covered by the data? (if applicable)</t>
+  </si>
+  <si>
+    <t>&lt;gmd:MD_SpatialRepresentationTypeCode</t>
+  </si>
+  <si>
+    <t>&lt;gmd:spatialRepresentationType&gt;</t>
+  </si>
+  <si>
+    <t>Drop-down list from codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_SpatialRepresentationTypeCode"</t>
+  </si>
+  <si>
+    <t>Spatial Data Type</t>
+  </si>
+  <si>
+    <t>Value for List: vector, grid, table or text, triangulated irregular network, stereographic imaging, video recording of a scene. For ISO: vector, grid, tin, stereoModel, video</t>
+  </si>
+  <si>
+    <t>How are your data represented in space? Through a vector spatial representation, a spatial grid of values, a table, a video of a scene, etc.?</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>What is the format of your data that is available for distribution?</t>
+  </si>
+  <si>
+    <t>gmd:MD_Format</t>
+  </si>
+  <si>
+    <t>Drop-down list, plus write-in option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values for List: </t>
   </si>
 </sst>
 </file>
@@ -660,7 +708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,7 +722,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -844,8 +892,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -901,8 +955,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -913,11 +976,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1002,6 +1065,9 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1086,6 +1152,9 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1418,13 +1487,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="T20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="S30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1454,14 +1523,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1544,16 +1613,16 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="24" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1571,7 +1640,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="23" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1588,10 +1657,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1607,7 +1676,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="20"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1625,11 +1694,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1650,7 +1719,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="20"/>
+      <c r="M5" s="23"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1662,11 +1731,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1680,7 +1749,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="20"/>
+      <c r="M6" s="23"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1695,11 +1764,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1713,7 +1782,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="20"/>
+      <c r="M7" s="23"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1722,12 +1791,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="20" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1742,7 +1811,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="20"/>
+      <c r="M8" s="23"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1757,12 +1826,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="20"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1844,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="20"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1790,12 +1859,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="20"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1808,7 +1877,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="20"/>
+      <c r="M10" s="23"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1820,12 +1889,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="20"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1838,7 +1907,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="20"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1856,12 +1925,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="20"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1874,7 +1943,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="20"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1886,12 +1955,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="20"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1904,7 +1973,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="20"/>
+      <c r="M13" s="23"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1922,12 +1991,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1940,7 +2009,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="20"/>
+      <c r="M14" s="23"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1955,12 +2024,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1973,7 +2042,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="20"/>
+      <c r="M15" s="23"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1985,9 +2054,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -2006,7 +2075,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="M16" s="23" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2020,9 +2089,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2041,7 +2110,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="20"/>
+      <c r="M17" s="23"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2056,10 +2125,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="20" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2077,7 +2146,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="20"/>
+      <c r="M18" s="23"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2098,10 +2167,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="20"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2117,7 +2186,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="20"/>
+      <c r="M19" s="23"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2138,9 +2207,9 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
@@ -2156,7 +2225,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="20"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2179,15 +2248,15 @@
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="105">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="G21" s="19" t="s">
-        <v>182</v>
+    <row r="21" spans="1:23" ht="75">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="G21" s="20" t="s">
+        <v>198</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>38</v>
@@ -2198,90 +2267,87 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="20"/>
+      <c r="M21" s="23"/>
       <c r="N21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="105">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="G22" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="23"/>
+      <c r="N22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="T21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U21" s="2" t="s">
+      <c r="T22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="V21" s="2" t="s">
+      <c r="V22" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="90">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="20" t="s">
+    <row r="23" spans="1:23" ht="90">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="2" t="s">
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" s="20"/>
-      <c r="N22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="45">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="20"/>
+      <c r="M23" s="23"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2291,9 +2357,6 @@
       <c r="Q23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="S23" s="2" t="s">
         <v>118</v>
       </c>
@@ -2304,40 +2367,43 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="90">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20" t="s">
-        <v>33</v>
-      </c>
+    <row r="24" spans="1:23" ht="45">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="R24" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="S24" s="2" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>7</v>
@@ -2345,46 +2411,61 @@
       <c r="U24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="W24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:23" ht="90">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W25" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="2" t="s">
+    <row r="26" spans="1:23">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M25" s="20"/>
-      <c r="S25" s="2">
-        <v>-117.531786</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>41</v>
@@ -2395,23 +2476,23 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="20"/>
+      <c r="M26" s="23"/>
       <c r="S26" s="2">
-        <v>-110.655421</v>
+        <v>-117.531786</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>41</v>
@@ -2422,23 +2503,23 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="20"/>
+      <c r="M27" s="23"/>
       <c r="S27" s="2">
-        <v>41.946097000000002</v>
+        <v>-110.655421</v>
       </c>
       <c r="T27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>41</v>
@@ -2449,73 +2530,76 @@
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="20"/>
+      <c r="M28" s="23"/>
       <c r="S28" s="2">
+        <v>41.946097000000002</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="23"/>
+      <c r="S29" s="2">
         <v>49.039541999999997</v>
       </c>
-      <c r="T28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="30">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20" t="s">
+      <c r="T29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="30">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="10" t="s">
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M29" s="20"/>
-      <c r="T29" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="2" t="s">
+      <c r="J30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="T30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="20"/>
-      <c r="T30" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>39</v>
@@ -2526,277 +2610,255 @@
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="20"/>
+      <c r="M31" s="23"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="85" customHeight="1">
-      <c r="A32" s="21"/>
-      <c r="B32" s="20" t="s">
+    <row r="32" spans="1:23">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="T32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="30">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="23"/>
+      <c r="T33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="23"/>
+      <c r="T34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="23"/>
+      <c r="T35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="85" customHeight="1">
+      <c r="A36" s="24"/>
+      <c r="B36" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C36" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D36" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E36" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="10" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" s="2" t="s">
+      <c r="I36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="M36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="R32" s="2" t="s">
+      <c r="R36" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="T32" s="2" t="s">
+      <c r="T36" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="U36" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="W32" s="2" t="s">
+      <c r="W36" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="30" customHeight="1">
-      <c r="A33" s="21"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="10" t="s">
+    <row r="37" spans="1:23" ht="30" customHeight="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="20" t="s">
+      <c r="J37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="N33" s="12" t="s">
+      <c r="N37" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="T33" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="30">
-      <c r="A34" s="21"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="2" t="s">
+      <c r="T37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="30">
+      <c r="A38" s="24"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="20"/>
-      <c r="N34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
-      <c r="A35" s="21"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" s="20"/>
-      <c r="N35" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="30">
-      <c r="A36" s="21"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="20"/>
-      <c r="N36" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="30">
-      <c r="A37" s="21"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="20"/>
-      <c r="N37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="30">
-      <c r="A38" s="21"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="J38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="20"/>
+      <c r="M38" s="23"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="T38" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="30">
-      <c r="A39" s="21"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="20"/>
+    <row r="39" spans="1:23">
+      <c r="A39" s="24"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="23" t="s">
+        <v>16</v>
+      </c>
       <c r="G39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M39" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="M39" s="23"/>
       <c r="N39" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="T39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="30">
-      <c r="A40" s="21"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="20"/>
+    <row r="40" spans="1:23" ht="30">
+      <c r="A40" s="24"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="2" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>37</v>
@@ -2807,62 +2869,59 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="20"/>
+      <c r="M40" s="23"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="45">
-      <c r="A41" s="21"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="20"/>
+    <row r="41" spans="1:23" ht="30">
+      <c r="A41" s="24"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="20"/>
+      <c r="M41" s="23"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="T41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="30">
-      <c r="A42" s="21"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="20"/>
+    <row r="42" spans="1:23" ht="30">
+      <c r="A42" s="24"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="23"/>
       <c r="G42" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>6</v>
@@ -2870,68 +2929,59 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="20"/>
+      <c r="M42" s="23"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="T42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="90">
-      <c r="A43" s="21"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="22"/>
-      <c r="G43" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>146</v>
+    <row r="43" spans="1:23" ht="30">
+      <c r="A43" s="24"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M43" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="M43" s="23"/>
       <c r="N43" s="2" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="30">
-      <c r="A44" s="21"/>
-      <c r="B44" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="15"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="30">
+      <c r="A44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="23"/>
       <c r="G44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>6</v>
@@ -2939,77 +2989,62 @@
       <c r="K44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="M44" s="23"/>
       <c r="N44" s="2" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="30">
-      <c r="A45" s="21"/>
-      <c r="B45" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" s="15"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="45">
+      <c r="A45" s="24"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="23"/>
       <c r="G45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>150</v>
+        <v>15</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M45" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="M45" s="23"/>
       <c r="N45" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="B46" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>150</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="30">
+      <c r="A46" s="24"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>6</v>
@@ -3017,37 +3052,32 @@
       <c r="K46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M46" s="4" t="s">
-        <v>151</v>
+      <c r="M46" s="23"/>
+      <c r="N46" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U46" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="B47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>150</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="30">
+      <c r="A47" s="24"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>6</v>
@@ -3055,75 +3085,74 @@
       <c r="K47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M47" s="4" t="s">
-        <v>151</v>
+      <c r="M47" s="19"/>
+      <c r="N47" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>28</v>
+        <v>203</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
-      <c r="B48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="V47" s="26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="90">
+      <c r="A48" s="24"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="25"/>
+      <c r="G48" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>151</v>
+        <v>109</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R48" s="2" t="s">
-        <v>160</v>
+        <v>99</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" ht="45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="30">
+      <c r="A49" s="24"/>
       <c r="B49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>150</v>
+        <v>94</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="G49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>6</v>
@@ -3132,39 +3161,35 @@
         <v>7</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="T49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W49" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="30">
+      <c r="A50" s="24"/>
       <c r="B50" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="G50" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>150</v>
@@ -3182,33 +3207,27 @@
         <v>57</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R50" s="2">
-        <v>2003</v>
-      </c>
       <c r="T50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W50" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
       <c r="B51" s="3" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="H51" s="14" t="s">
         <v>150</v>
@@ -3222,8 +3241,17 @@
       <c r="M51" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="O51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R51" s="2" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="T51" s="2" t="s">
         <v>7</v>
@@ -3232,12 +3260,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="2:23" ht="75">
+    <row r="52" spans="1:23">
       <c r="B52" s="3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>150</v>
@@ -3251,8 +3279,17 @@
       <c r="M52" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="O52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R52" s="2" t="s">
-        <v>174</v>
+        <v>28</v>
       </c>
       <c r="T52" s="2" t="s">
         <v>7</v>
@@ -3261,41 +3298,227 @@
         <v>161</v>
       </c>
     </row>
+    <row r="53" spans="1:23">
+      <c r="B53" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R53" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U53" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" ht="45">
+      <c r="B54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W54" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="45">
+      <c r="B55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R55" s="2">
+        <v>2003</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
+      <c r="B56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="75">
+      <c r="B57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U57" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
+    <mergeCell ref="M37:M46"/>
+    <mergeCell ref="A3:A50"/>
+    <mergeCell ref="B3:B35"/>
+    <mergeCell ref="M3:M15"/>
+    <mergeCell ref="M25:M35"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="M16:M24"/>
+    <mergeCell ref="D36:D48"/>
+    <mergeCell ref="F39:F46"/>
+    <mergeCell ref="C36:C48"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="E36:E48"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="E33:E35"/>
     <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F25:F29"/>
     <mergeCell ref="F8:F15"/>
     <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="C3:C31"/>
-    <mergeCell ref="M33:M42"/>
-    <mergeCell ref="A3:A45"/>
-    <mergeCell ref="B3:B31"/>
-    <mergeCell ref="M3:M15"/>
-    <mergeCell ref="M24:M31"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M16:M23"/>
-    <mergeCell ref="D32:D43"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="C32:C43"/>
-    <mergeCell ref="B32:B43"/>
-    <mergeCell ref="E32:E43"/>
+    <mergeCell ref="D25:D35"/>
+    <mergeCell ref="C3:C35"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="21" fitToHeight="2" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="28" max="16383" man="1"/>
-    <brk id="44" max="16383" man="1"/>
+    <brk id="32" max="16383" man="1"/>
+    <brk id="49" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>

</xml_diff>

<commit_message>
updated design doc xlsx to latest
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="-4140" windowWidth="11120" windowHeight="20360" tabRatio="500"/>
+    <workbookView xWindow="33580" yWindow="-3980" windowWidth="30980" windowHeight="20200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$50</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$G:$G,Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="206">
   <si>
     <t>Required?</t>
   </si>
@@ -532,18 +532,6 @@
     <t>uuid to be generated by metadata system</t>
   </si>
   <si>
-    <t>uuid linked to NKN Portal data record</t>
-  </si>
-  <si>
-    <t>Dataset URI</t>
-  </si>
-  <si>
-    <t>Dataset Uri</t>
-  </si>
-  <si>
-    <t>gmd:dataSetURI</t>
-  </si>
-  <si>
     <t>Metadata Constraints</t>
   </si>
   <si>
@@ -568,6 +556,9 @@
     <t>gmd:MD_SCopeCode</t>
   </si>
   <si>
+    <t>Is the data you are describing with this metadata a single dataset or a collectiion of datasets that have the same specification. Example: A climate data series include the same variables but over 1 year at one day intervals; this series would contain 365 datasets.</t>
+  </si>
+  <si>
     <t>Idaho, USA</t>
   </si>
   <si>
@@ -577,9 +568,6 @@
     <t>gmd: language</t>
   </si>
   <si>
-    <t>connect to NKN datastore</t>
-  </si>
-  <si>
     <t>What is the status of your dataset? For example, is it complete (you anticipate no further work and consider it final) or is it ongoing (continually being updated)?</t>
   </si>
   <si>
@@ -592,16 +580,67 @@
     <t>Drop-down list from ISO codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_MaintenanceFrequencyCode"</t>
   </si>
   <si>
+    <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are availabel if you do not plan to update your data or do not know the specific frequency of updates.</t>
+  </si>
+  <si>
     <t>Values for List: completed, continually updated, in process, planned, needs to be generated or updated, stored in an offline facility, no longer valid. ISO values for xml: completed, onGoing, underDevelopment, planned, required, historicalArchive, obsolete</t>
   </si>
   <si>
     <t>Value for List: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, as needed, irregular, not planned, unknown   For ISO: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, asNeeded, irregular, notPlanned, unknown</t>
   </si>
   <si>
-    <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are available if you do not plan to update your data or do not know the specific frequency of updates.</t>
-  </si>
-  <si>
-    <t>Is the data you are describing with this metadata a single dataset or a collection of datasets that have the same specification. Example: A climate data series include the same variables but over 1 year at one-day intervals; this series would contain 365 datasets.</t>
+    <t>Dropdown list</t>
+  </si>
+  <si>
+    <t>Values for List: dataset, series     ISO Values for xml: [same]</t>
+  </si>
+  <si>
+    <t>Needs to be editable; even if NKN is choosen as distributor</t>
+  </si>
+  <si>
+    <t>Vertical Extent</t>
+  </si>
+  <si>
+    <t>Vertical Minimum</t>
+  </si>
+  <si>
+    <t>Vertical Maximum</t>
+  </si>
+  <si>
+    <t>What is the minimum and maximum vertical heights covered by the data? (if applicable)</t>
+  </si>
+  <si>
+    <t>&lt;gmd:MD_SpatialRepresentationTypeCode</t>
+  </si>
+  <si>
+    <t>&lt;gmd:spatialRepresentationType&gt;</t>
+  </si>
+  <si>
+    <t>Drop-down list from codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_SpatialRepresentationTypeCode"</t>
+  </si>
+  <si>
+    <t>Spatial Data Type</t>
+  </si>
+  <si>
+    <t>Value for List: vector, grid, table or text, triangulated irregular network, stereographic imaging, video recording of a scene. For ISO: vector, grid, tin, stereoModel, video</t>
+  </si>
+  <si>
+    <t>How are your data represented in space? Through a vector spatial representation, a spatial grid of values, a table, a video of a scene, etc.?</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>What is the format of your data that is available for distribution?</t>
+  </si>
+  <si>
+    <t>gmd:MD_Format</t>
+  </si>
+  <si>
+    <t>Drop-down list, plus write-in option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values for List: </t>
   </si>
 </sst>
 </file>
@@ -669,7 +708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,7 +722,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -843,8 +882,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -900,7 +955,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -915,8 +976,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -996,6 +1060,14 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1075,6 +1147,14 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1407,22 +1487,21 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="V20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="S30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
+      <selection pane="bottomRight" activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="38.33203125" style="10" customWidth="1"/>
@@ -1444,14 +1523,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1512,13 +1591,13 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -1526,18 +1605,24 @@
       <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="U2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="24" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1555,7 +1640,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="23" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1572,10 +1657,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1591,7 +1676,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1609,11 +1694,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1634,7 +1719,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="23"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1646,11 +1731,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1664,7 +1749,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="21"/>
+      <c r="M6" s="23"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1679,11 +1764,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1697,7 +1782,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="21"/>
+      <c r="M7" s="23"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1706,12 +1791,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1726,7 +1811,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="23"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1741,12 +1826,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="21"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1759,7 +1844,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1774,12 +1859,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1792,7 +1877,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="21"/>
+      <c r="M10" s="23"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1804,12 +1889,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1822,7 +1907,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="21"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1840,12 +1925,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1858,7 +1943,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="21"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1870,12 +1955,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1888,7 +1973,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="21"/>
+      <c r="M13" s="23"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1906,12 +1991,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1924,7 +2009,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="21"/>
+      <c r="M14" s="23"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1939,12 +2024,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1957,7 +2042,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="21"/>
+      <c r="M15" s="23"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1969,9 +2054,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1990,7 +2075,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="23" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2004,9 +2089,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2025,7 +2110,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="21"/>
+      <c r="M17" s="23"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2040,10 +2125,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2061,7 +2146,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="21"/>
+      <c r="M18" s="23"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2082,10 +2167,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2101,7 +2186,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="21"/>
+      <c r="M19" s="23"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2112,7 +2197,7 @@
         <v>98</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="T19" s="2" t="s">
         <v>6</v>
@@ -2122,14 +2207,14 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>38</v>
@@ -2140,7 +2225,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="21"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2160,18 +2245,18 @@
         <v>140</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="105">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="G21" s="19" t="s">
         <v>186</v>
       </c>
+    </row>
+    <row r="21" spans="1:23" ht="75">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="G21" s="20" t="s">
+        <v>198</v>
+      </c>
       <c r="H21" s="10" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>38</v>
@@ -2182,90 +2267,87 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="21"/>
+      <c r="M21" s="23"/>
       <c r="N21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="105">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="G22" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="23"/>
+      <c r="N22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="90">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21" t="s">
+    </row>
+    <row r="23" spans="1:23" ht="90">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="2" t="s">
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" s="21"/>
-      <c r="N22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="45">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="21"/>
+      <c r="M23" s="23"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2275,9 +2357,6 @@
       <c r="Q23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="S23" s="2" t="s">
         <v>118</v>
       </c>
@@ -2288,40 +2367,43 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="90">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
-        <v>33</v>
-      </c>
+    <row r="24" spans="1:23" ht="45">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="R24" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="S24" s="2" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>7</v>
@@ -2329,458 +2411,454 @@
       <c r="U24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="W24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:23" ht="90">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W25" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="2" t="s">
+    <row r="26" spans="1:23">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M25" s="21"/>
-      <c r="S25" s="2">
-        <v>-117.531786</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="21"/>
+      <c r="M26" s="23"/>
       <c r="S26" s="2">
-        <v>-110.655421</v>
+        <v>-117.531786</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="21"/>
+      <c r="M27" s="23"/>
       <c r="S27" s="2">
-        <v>41.946097000000002</v>
+        <v>-110.655421</v>
       </c>
       <c r="T27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="21"/>
+      <c r="M28" s="23"/>
       <c r="S28" s="2">
+        <v>41.946097000000002</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="23"/>
+      <c r="S29" s="2">
         <v>49.039541999999997</v>
       </c>
-      <c r="T28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="30">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
+      <c r="T29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="30">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="10" t="s">
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="T29" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="2" t="s">
+      <c r="J30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="T30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="21"/>
-      <c r="T30" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="21"/>
+      <c r="M31" s="23"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="85" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="21" t="s">
+    <row r="32" spans="1:23">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="T32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="30">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="23"/>
+      <c r="T33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="23"/>
+      <c r="T34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="23"/>
+      <c r="T35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="85" customHeight="1">
+      <c r="A36" s="24"/>
+      <c r="B36" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C36" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D36" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E36" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="10" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="M32" s="4" t="s">
+      <c r="I36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="R32" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="T32" s="2" t="s">
+      <c r="R36" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="T36" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="U32" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="W32" s="2" t="s">
+      <c r="U36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W36" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="30" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="10" t="s">
+    <row r="37" spans="1:23" ht="30" customHeight="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="21" t="s">
+      <c r="J37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="N33" s="12" t="s">
+      <c r="N37" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="T33" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="30">
-      <c r="A34" s="22"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="2" t="s">
+      <c r="T37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="30">
+      <c r="A38" s="24"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="21"/>
-      <c r="N34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
-      <c r="A35" s="22"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" s="21"/>
-      <c r="N35" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="30">
-      <c r="A36" s="22"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="21"/>
-      <c r="N36" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="30">
-      <c r="A37" s="22"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="21"/>
-      <c r="N37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="30">
-      <c r="A38" s="22"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="J38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="21"/>
+      <c r="M38" s="23"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="T38" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="30">
-      <c r="A39" s="22"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="21"/>
+    <row r="39" spans="1:23">
+      <c r="A39" s="24"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="23" t="s">
+        <v>16</v>
+      </c>
       <c r="G39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M39" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="M39" s="23"/>
       <c r="N39" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="T39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="30">
-      <c r="A40" s="22"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="21"/>
+    <row r="40" spans="1:23" ht="30">
+      <c r="A40" s="24"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="2" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>37</v>
@@ -2791,62 +2869,59 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="21"/>
+      <c r="M40" s="23"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="45">
-      <c r="A41" s="22"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+    <row r="41" spans="1:23" ht="30">
+      <c r="A41" s="24"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="21"/>
+      <c r="M41" s="23"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="T41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="30">
-      <c r="A42" s="22"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+    <row r="42" spans="1:23" ht="30">
+      <c r="A42" s="24"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="23"/>
       <c r="G42" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>6</v>
@@ -2854,68 +2929,59 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="21"/>
+      <c r="M42" s="23"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="T42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="90">
-      <c r="A43" s="22"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="23"/>
-      <c r="G43" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>146</v>
+    <row r="43" spans="1:23" ht="30">
+      <c r="A43" s="24"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M43" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="M43" s="23"/>
       <c r="N43" s="2" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="30">
-      <c r="A44" s="22"/>
-      <c r="B44" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="15"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="30">
+      <c r="A44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="23"/>
       <c r="G44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>6</v>
@@ -2923,77 +2989,62 @@
       <c r="K44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="M44" s="23"/>
       <c r="N44" s="2" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="30">
-      <c r="A45" s="22"/>
-      <c r="B45" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" s="15"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="45">
+      <c r="A45" s="24"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="23"/>
       <c r="G45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>150</v>
+        <v>15</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M45" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="M45" s="23"/>
       <c r="N45" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="B46" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>150</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="30">
+      <c r="A46" s="24"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>6</v>
@@ -3001,37 +3052,32 @@
       <c r="K46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M46" s="4" t="s">
-        <v>151</v>
+      <c r="M46" s="23"/>
+      <c r="N46" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U46" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="B47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>150</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="30">
+      <c r="A47" s="24"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>6</v>
@@ -3039,75 +3085,74 @@
       <c r="K47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M47" s="4" t="s">
-        <v>151</v>
+      <c r="M47" s="19"/>
+      <c r="N47" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>28</v>
+        <v>203</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
-      <c r="B48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="V47" s="26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="90">
+      <c r="A48" s="24"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="25"/>
+      <c r="G48" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>151</v>
+        <v>109</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R48" s="2" t="s">
-        <v>160</v>
+        <v>99</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" ht="45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="30">
+      <c r="A49" s="24"/>
       <c r="B49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>150</v>
+        <v>94</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="G49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>6</v>
@@ -3116,39 +3161,35 @@
         <v>7</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="T49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W49" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="30">
+      <c r="A50" s="24"/>
       <c r="B50" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="G50" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>150</v>
@@ -3166,36 +3207,30 @@
         <v>57</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R50" s="2">
-        <v>2003</v>
-      </c>
       <c r="T50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W50" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
       <c r="B51" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>171</v>
+        <v>154</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>6</v>
@@ -3206,31 +3241,31 @@
       <c r="M51" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N51" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="O51" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="R51" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="T51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="2:23">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
       <c r="B52" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>150</v>
@@ -3244,8 +3279,17 @@
       <c r="M52" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="O52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R52" s="2" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="T52" s="2" t="s">
         <v>7</v>
@@ -3254,12 +3298,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="2:23" ht="75">
+    <row r="53" spans="1:23">
       <c r="B53" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H53" s="14" t="s">
         <v>150</v>
@@ -3273,8 +3317,17 @@
       <c r="M53" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="O53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R53" s="2" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="T53" s="2" t="s">
         <v>7</v>
@@ -3283,41 +3336,189 @@
         <v>161</v>
       </c>
     </row>
+    <row r="54" spans="1:23" ht="45">
+      <c r="B54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W54" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="45">
+      <c r="B55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R55" s="2">
+        <v>2003</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
+      <c r="B56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="75">
+      <c r="B57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U57" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="M33:M42"/>
-    <mergeCell ref="A3:A45"/>
-    <mergeCell ref="B3:B31"/>
+  <mergeCells count="27">
+    <mergeCell ref="M37:M46"/>
+    <mergeCell ref="A3:A50"/>
+    <mergeCell ref="B3:B35"/>
     <mergeCell ref="M3:M15"/>
-    <mergeCell ref="M24:M31"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="M25:M35"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M16:M23"/>
-    <mergeCell ref="D32:D43"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="C32:C43"/>
-    <mergeCell ref="B32:B43"/>
-    <mergeCell ref="E32:E43"/>
+    <mergeCell ref="M16:M24"/>
+    <mergeCell ref="D36:D48"/>
+    <mergeCell ref="F39:F46"/>
+    <mergeCell ref="C36:C48"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="E36:E48"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="E33:E35"/>
     <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F25:F29"/>
     <mergeCell ref="F8:F15"/>
     <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="C3:C31"/>
+    <mergeCell ref="D25:D35"/>
+    <mergeCell ref="C3:C35"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="21" fitToHeight="2" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="28" max="16383" man="1"/>
-    <brk id="44" max="16383" man="1"/>
+    <brk id="32" max="16383" man="1"/>
+    <brk id="49" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>

</xml_diff>

<commit_message>
contact forms working properly
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31920" yWindow="-4140" windowWidth="11120" windowHeight="20360" tabRatio="500"/>
+    <workbookView xWindow="33580" yWindow="-3980" windowWidth="30980" windowHeight="20200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$50</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$G:$G,Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="206">
   <si>
     <t>Required?</t>
   </si>
@@ -532,18 +532,6 @@
     <t>uuid to be generated by metadata system</t>
   </si>
   <si>
-    <t>uuid linked to NKN Portal data record</t>
-  </si>
-  <si>
-    <t>Dataset URI</t>
-  </si>
-  <si>
-    <t>Dataset Uri</t>
-  </si>
-  <si>
-    <t>gmd:dataSetURI</t>
-  </si>
-  <si>
     <t>Metadata Constraints</t>
   </si>
   <si>
@@ -568,6 +556,9 @@
     <t>gmd:MD_SCopeCode</t>
   </si>
   <si>
+    <t>Is the data you are describing with this metadata a single dataset or a collectiion of datasets that have the same specification. Example: A climate data series include the same variables but over 1 year at one day intervals; this series would contain 365 datasets.</t>
+  </si>
+  <si>
     <t>Idaho, USA</t>
   </si>
   <si>
@@ -577,9 +568,6 @@
     <t>gmd: language</t>
   </si>
   <si>
-    <t>connect to NKN datastore</t>
-  </si>
-  <si>
     <t>What is the status of your dataset? For example, is it complete (you anticipate no further work and consider it final) or is it ongoing (continually being updated)?</t>
   </si>
   <si>
@@ -592,16 +580,67 @@
     <t>Drop-down list from ISO codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_MaintenanceFrequencyCode"</t>
   </si>
   <si>
+    <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are availabel if you do not plan to update your data or do not know the specific frequency of updates.</t>
+  </si>
+  <si>
     <t>Values for List: completed, continually updated, in process, planned, needs to be generated or updated, stored in an offline facility, no longer valid. ISO values for xml: completed, onGoing, underDevelopment, planned, required, historicalArchive, obsolete</t>
   </si>
   <si>
     <t>Value for List: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, as needed, irregular, not planned, unknown   For ISO: continual, daily, weekly, fortnightly, monthly, quarterly, biannually, annually, asNeeded, irregular, notPlanned, unknown</t>
   </si>
   <si>
-    <t>Please select the frequency with which changes (any modifications and deletions) are or will be made to your data after it is produced? Please select a value from below. Options are available if you do not plan to update your data or do not know the specific frequency of updates.</t>
-  </si>
-  <si>
-    <t>Is the data you are describing with this metadata a single dataset or a collection of datasets that have the same specification. Example: A climate data series include the same variables but over 1 year at one-day intervals; this series would contain 365 datasets.</t>
+    <t>Dropdown list</t>
+  </si>
+  <si>
+    <t>Values for List: dataset, series     ISO Values for xml: [same]</t>
+  </si>
+  <si>
+    <t>Needs to be editable; even if NKN is choosen as distributor</t>
+  </si>
+  <si>
+    <t>Vertical Extent</t>
+  </si>
+  <si>
+    <t>Vertical Minimum</t>
+  </si>
+  <si>
+    <t>Vertical Maximum</t>
+  </si>
+  <si>
+    <t>What is the minimum and maximum vertical heights covered by the data? (if applicable)</t>
+  </si>
+  <si>
+    <t>&lt;gmd:MD_SpatialRepresentationTypeCode</t>
+  </si>
+  <si>
+    <t>&lt;gmd:spatialRepresentationType&gt;</t>
+  </si>
+  <si>
+    <t>Drop-down list from codeList="http://www.isotc211.org/2005/resources/Codelist/gmxCodelists.xml#MD_SpatialRepresentationTypeCode"</t>
+  </si>
+  <si>
+    <t>Spatial Data Type</t>
+  </si>
+  <si>
+    <t>Value for List: vector, grid, table or text, triangulated irregular network, stereographic imaging, video recording of a scene. For ISO: vector, grid, tin, stereoModel, video</t>
+  </si>
+  <si>
+    <t>How are your data represented in space? Through a vector spatial representation, a spatial grid of values, a table, a video of a scene, etc.?</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>What is the format of your data that is available for distribution?</t>
+  </si>
+  <si>
+    <t>gmd:MD_Format</t>
+  </si>
+  <si>
+    <t>Drop-down list, plus write-in option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values for List: </t>
   </si>
 </sst>
 </file>
@@ -669,7 +708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,7 +722,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -843,8 +882,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -900,7 +955,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -915,8 +976,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="175">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -996,6 +1060,14 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1075,6 +1147,14 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1407,22 +1487,21 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="V20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="S30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V20" sqref="V20"/>
+      <selection pane="bottomRight" activeCell="V48" sqref="V48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="38.33203125" style="10" customWidth="1"/>
@@ -1444,14 +1523,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1512,13 +1591,13 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="17" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
@@ -1526,18 +1605,24 @@
       <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="U2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="24" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1555,7 +1640,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="23" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1572,10 +1657,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1591,7 +1676,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="23"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1609,11 +1694,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1634,7 +1719,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="23"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1646,11 +1731,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1664,7 +1749,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="21"/>
+      <c r="M6" s="23"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1679,11 +1764,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1697,7 +1782,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="21"/>
+      <c r="M7" s="23"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1706,12 +1791,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="21" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="23" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1726,7 +1811,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="23"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1741,12 +1826,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="21"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1759,7 +1844,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="23"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1774,12 +1859,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="21"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1792,7 +1877,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="21"/>
+      <c r="M10" s="23"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1804,12 +1889,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="21"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1822,7 +1907,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="21"/>
+      <c r="M11" s="23"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1840,12 +1925,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="21"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="23"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1858,7 +1943,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="21"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1870,12 +1955,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="21"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="23"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1888,7 +1973,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="21"/>
+      <c r="M13" s="23"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1906,12 +1991,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="21"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -1924,7 +2009,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="21"/>
+      <c r="M14" s="23"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -1939,12 +2024,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="23"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1957,7 +2042,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="21"/>
+      <c r="M15" s="23"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -1969,9 +2054,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -1990,7 +2075,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="23" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2004,9 +2089,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2025,7 +2110,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="21"/>
+      <c r="M17" s="23"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2040,10 +2125,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2061,7 +2146,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="21"/>
+      <c r="M18" s="23"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2082,10 +2167,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="23"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2101,7 +2186,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="21"/>
+      <c r="M19" s="23"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2112,7 +2197,7 @@
         <v>98</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="T19" s="2" t="s">
         <v>6</v>
@@ -2122,14 +2207,14 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>38</v>
@@ -2140,7 +2225,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="21"/>
+      <c r="M20" s="23"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2160,18 +2245,18 @@
         <v>140</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="105">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="G21" s="19" t="s">
         <v>186</v>
       </c>
+    </row>
+    <row r="21" spans="1:23" ht="75">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="G21" s="20" t="s">
+        <v>198</v>
+      </c>
       <c r="H21" s="10" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>38</v>
@@ -2182,90 +2267,87 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="21"/>
+      <c r="M21" s="23"/>
       <c r="N21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="105">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="G22" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" s="23"/>
+      <c r="N22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="V22" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="V21" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="90">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21" t="s">
+    </row>
+    <row r="23" spans="1:23" ht="90">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="2" t="s">
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M22" s="21"/>
-      <c r="N22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="45">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="21"/>
+      <c r="M23" s="23"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2275,9 +2357,6 @@
       <c r="Q23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="S23" s="2" t="s">
         <v>118</v>
       </c>
@@ -2288,40 +2367,43 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="90">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21" t="s">
-        <v>33</v>
-      </c>
+    <row r="24" spans="1:23" ht="45">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="2" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>108</v>
+        <v>7</v>
+      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="R24" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="S24" s="2" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>7</v>
@@ -2329,458 +2411,454 @@
       <c r="U24" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="W24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:23" ht="90">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W25" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="2" t="s">
+    <row r="26" spans="1:23">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M25" s="21"/>
-      <c r="S25" s="2">
-        <v>-117.531786</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="22"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="21"/>
+      <c r="M26" s="23"/>
       <c r="S26" s="2">
-        <v>-110.655421</v>
+        <v>-117.531786</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="21"/>
+      <c r="M27" s="23"/>
       <c r="S27" s="2">
-        <v>41.946097000000002</v>
+        <v>-110.655421</v>
       </c>
       <c r="T27" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="22"/>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="21"/>
+      <c r="M28" s="23"/>
       <c r="S28" s="2">
+        <v>41.946097000000002</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="23"/>
+      <c r="S29" s="2">
         <v>49.039541999999997</v>
       </c>
-      <c r="T28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="30">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21" t="s">
+      <c r="T29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="30">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="10" t="s">
+      <c r="G30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M29" s="21"/>
-      <c r="T29" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="A30" s="22"/>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="2" t="s">
+      <c r="J30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="T30" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="21"/>
-      <c r="T30" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="22"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="21"/>
+      <c r="M31" s="23"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="85" customHeight="1">
-      <c r="A32" s="22"/>
-      <c r="B32" s="21" t="s">
+    <row r="32" spans="1:23">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M32" s="23"/>
+      <c r="T32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" ht="30">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M33" s="23"/>
+      <c r="T33" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M34" s="23"/>
+      <c r="T34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M35" s="23"/>
+      <c r="T35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="85" customHeight="1">
+      <c r="A36" s="24"/>
+      <c r="B36" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C36" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D36" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E36" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="10" t="s">
+      <c r="F36" s="2"/>
+      <c r="G36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="I32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="M32" s="4" t="s">
+      <c r="I36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="R32" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="T32" s="2" t="s">
+      <c r="R36" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="T36" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="U32" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="W32" s="2" t="s">
+      <c r="U36" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="W36" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="30" customHeight="1">
-      <c r="A33" s="22"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="10" t="s">
+    <row r="37" spans="1:23" ht="30" customHeight="1">
+      <c r="A37" s="24"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="21" t="s">
+      <c r="J37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="N33" s="12" t="s">
+      <c r="N37" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="T33" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="30">
-      <c r="A34" s="22"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="2" t="s">
+      <c r="T37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="30">
+      <c r="A38" s="24"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="21"/>
-      <c r="N34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="T34" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
-      <c r="A35" s="22"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M35" s="21"/>
-      <c r="N35" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T35" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="30">
-      <c r="A36" s="22"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="21"/>
-      <c r="N36" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="T36" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="30">
-      <c r="A37" s="22"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="21"/>
-      <c r="N37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="T37" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="30">
-      <c r="A38" s="22"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="J38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="21"/>
+      <c r="M38" s="23"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="T38" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="30">
-      <c r="A39" s="22"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="21"/>
+    <row r="39" spans="1:23">
+      <c r="A39" s="24"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="23" t="s">
+        <v>16</v>
+      </c>
       <c r="G39" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M39" s="21"/>
+        <v>11</v>
+      </c>
+      <c r="M39" s="23"/>
       <c r="N39" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="T39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="30">
-      <c r="A40" s="22"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="21"/>
+    <row r="40" spans="1:23" ht="30">
+      <c r="A40" s="24"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="23"/>
       <c r="G40" s="2" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>37</v>
@@ -2791,62 +2869,59 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="21"/>
+      <c r="M40" s="23"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="45">
-      <c r="A41" s="22"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="21"/>
+    <row r="41" spans="1:23" ht="30">
+      <c r="A41" s="24"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="23"/>
       <c r="G41" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="21"/>
+      <c r="M41" s="23"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="T41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="30">
-      <c r="A42" s="22"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="21"/>
+    <row r="42" spans="1:23" ht="30">
+      <c r="A42" s="24"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="23"/>
       <c r="G42" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>6</v>
@@ -2854,68 +2929,59 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="21"/>
+      <c r="M42" s="23"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="T42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="90">
-      <c r="A43" s="22"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="23"/>
-      <c r="G43" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>146</v>
+    <row r="43" spans="1:23" ht="30">
+      <c r="A43" s="24"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>147</v>
+        <v>41</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M43" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="M43" s="23"/>
       <c r="N43" s="2" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="T43" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="30">
-      <c r="A44" s="22"/>
-      <c r="B44" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="15"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="30">
+      <c r="A44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="23"/>
       <c r="G44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>6</v>
@@ -2923,77 +2989,62 @@
       <c r="K44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="M44" s="23"/>
       <c r="N44" s="2" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U44" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="30">
-      <c r="A45" s="22"/>
-      <c r="B45" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" s="15"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="45">
+      <c r="A45" s="24"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="23"/>
       <c r="G45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>150</v>
+        <v>15</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M45" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="M45" s="23"/>
       <c r="N45" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="T45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U45" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="B46" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H46" s="14" t="s">
-        <v>150</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="30">
+      <c r="A46" s="24"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>6</v>
@@ -3001,37 +3052,32 @@
       <c r="K46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M46" s="4" t="s">
-        <v>151</v>
+      <c r="M46" s="23"/>
+      <c r="N46" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R46" s="2" t="s">
-        <v>156</v>
+        <v>75</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U46" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="B47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>150</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="30">
+      <c r="A47" s="24"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>6</v>
@@ -3039,75 +3085,74 @@
       <c r="K47" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M47" s="4" t="s">
-        <v>151</v>
+      <c r="M47" s="19"/>
+      <c r="N47" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="Q47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R47" s="2" t="s">
-        <v>28</v>
+        <v>203</v>
       </c>
       <c r="T47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
-      <c r="B48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>150</v>
+        <v>6</v>
+      </c>
+      <c r="V47" s="26" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="90">
+      <c r="A48" s="24"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="25"/>
+      <c r="G48" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>151</v>
+        <v>109</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R48" s="2" t="s">
-        <v>160</v>
+        <v>99</v>
+      </c>
+      <c r="P48" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U48" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" ht="45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="30">
+      <c r="A49" s="24"/>
       <c r="B49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>150</v>
+        <v>94</v>
+      </c>
+      <c r="E49" s="15"/>
+      <c r="G49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>6</v>
@@ -3116,39 +3161,35 @@
         <v>7</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>166</v>
+        <v>24</v>
       </c>
       <c r="T49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W49" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="30">
+      <c r="A50" s="24"/>
       <c r="B50" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>163</v>
+        <v>148</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="G50" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>150</v>
@@ -3166,36 +3207,30 @@
         <v>57</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R50" s="2">
-        <v>2003</v>
-      </c>
       <c r="T50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W50" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="2:23" ht="30">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23">
       <c r="B51" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>171</v>
+        <v>154</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>6</v>
@@ -3206,31 +3241,31 @@
       <c r="M51" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="N51" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="O51" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="R51" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="T51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="2:23">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23">
       <c r="B52" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>150</v>
@@ -3244,8 +3279,17 @@
       <c r="M52" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="O52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R52" s="2" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="T52" s="2" t="s">
         <v>7</v>
@@ -3254,12 +3298,12 @@
         <v>161</v>
       </c>
     </row>
-    <row r="53" spans="2:23" ht="75">
+    <row r="53" spans="1:23">
       <c r="B53" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H53" s="14" t="s">
         <v>150</v>
@@ -3273,8 +3317,17 @@
       <c r="M53" s="4" t="s">
         <v>151</v>
       </c>
+      <c r="O53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R53" s="2" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="T53" s="2" t="s">
         <v>7</v>
@@ -3283,41 +3336,189 @@
         <v>161</v>
       </c>
     </row>
+    <row r="54" spans="1:23" ht="45">
+      <c r="B54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W54" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="45">
+      <c r="B55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R55" s="2">
+        <v>2003</v>
+      </c>
+      <c r="T55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U55" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="W55" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23">
+      <c r="B56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R56" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U56" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" ht="75">
+      <c r="B57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U57" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="M33:M42"/>
-    <mergeCell ref="A3:A45"/>
-    <mergeCell ref="B3:B31"/>
+  <mergeCells count="27">
+    <mergeCell ref="M37:M46"/>
+    <mergeCell ref="A3:A50"/>
+    <mergeCell ref="B3:B35"/>
     <mergeCell ref="M3:M15"/>
-    <mergeCell ref="M24:M31"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="M25:M35"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="M16:M23"/>
-    <mergeCell ref="D32:D43"/>
-    <mergeCell ref="F35:F42"/>
-    <mergeCell ref="C32:C43"/>
-    <mergeCell ref="B32:B43"/>
-    <mergeCell ref="E32:E43"/>
+    <mergeCell ref="M16:M24"/>
+    <mergeCell ref="D36:D48"/>
+    <mergeCell ref="F39:F46"/>
+    <mergeCell ref="C36:C48"/>
+    <mergeCell ref="B36:B48"/>
+    <mergeCell ref="E36:E48"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="E33:E35"/>
     <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F24:F28"/>
+    <mergeCell ref="F25:F29"/>
     <mergeCell ref="F8:F15"/>
     <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D24:D31"/>
-    <mergeCell ref="C3:C31"/>
+    <mergeCell ref="D25:D35"/>
+    <mergeCell ref="C3:C35"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="21" fitToHeight="2" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="28" max="16383" man="1"/>
-    <brk id="44" max="16383" man="1"/>
+    <brk id="32" max="16383" man="1"/>
+    <brk id="49" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>

</xml_diff>

<commit_message>
added data format list to design doc Excel document
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33580" yWindow="-3980" windowWidth="30980" windowHeight="20200" tabRatio="500"/>
+    <workbookView xWindow="42240" yWindow="-2460" windowWidth="22320" windowHeight="18680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="207">
   <si>
     <t>Required?</t>
   </si>
@@ -640,7 +640,11 @@
     <t>Drop-down list, plus write-in option</t>
   </si>
   <si>
-    <t xml:space="preserve">Values for List: </t>
+    <t>Values for List: ASCII, csv, DLG, docx, DRG, DWG, eps, ERDAS, Esri grid, Esri TIN, FASTA, FASTQ, GenBank, GeoJSON, GeoTIFF, GML, HDF, jpeg, KML, LAS, mp3, MrSID, netCDF, pdf, php, png, py, R, SDXF, Shapefile, SPSS, Stata, Tab, tiff, txt, VBS, wav, xls, xlsx, xml</t>
+  </si>
+  <si>
+    <t>Dropdown values plus Type In option
+Allow multiple selection</t>
   </si>
 </sst>
 </file>
@@ -693,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,12 +707,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,7 +720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="175">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -898,8 +896,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -964,9 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -976,11 +975,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="175">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1068,6 +1067,8 @@
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1155,6 +1156,8 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1490,10 +1493,10 @@
   <dimension ref="A1:W57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="S30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="T46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V48" sqref="V48"/>
+      <selection pane="bottomRight" activeCell="V47" sqref="V47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1523,14 +1526,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1613,16 +1616,16 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>82</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -1640,7 +1643,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="22" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1657,10 +1660,10 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
       <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
@@ -1676,7 +1679,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="23"/>
+      <c r="M4" s="22"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1694,11 +1697,11 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1719,7 +1722,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="23"/>
+      <c r="M5" s="22"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1731,11 +1734,11 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="7"/>
       <c r="G6" s="2" t="s">
         <v>10</v>
@@ -1749,7 +1752,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="23"/>
+      <c r="M6" s="22"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1764,11 +1767,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
         <v>124</v>
@@ -1782,7 +1785,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="23"/>
+      <c r="M7" s="22"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1791,12 +1794,12 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="24"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="23" t="s">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1811,7 +1814,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="23"/>
+      <c r="M8" s="22"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1826,12 +1829,12 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1844,7 +1847,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="23"/>
+      <c r="M9" s="22"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1859,12 +1862,12 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="23"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1877,7 +1880,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="23"/>
+      <c r="M10" s="22"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1889,12 +1892,12 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="23"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1907,7 +1910,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="23"/>
+      <c r="M11" s="22"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1925,12 +1928,12 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="23"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
@@ -1943,7 +1946,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="23"/>
+      <c r="M12" s="22"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1955,12 +1958,12 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="23"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="23"/>
+      <c r="M13" s="22"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1991,12 +1994,12 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="23"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="2" t="s">
         <v>15</v>
       </c>
@@ -2009,7 +2012,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="23"/>
+      <c r="M14" s="22"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -2024,12 +2027,12 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="23"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2042,7 +2045,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="23"/>
+      <c r="M15" s="22"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -2054,9 +2057,9 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
@@ -2075,7 +2078,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="22" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2089,9 +2092,9 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
@@ -2110,7 +2113,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="23"/>
+      <c r="M17" s="22"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2125,10 +2128,10 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="23" t="s">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="22" t="s">
         <v>84</v>
       </c>
       <c r="G18" s="8" t="s">
@@ -2146,7 +2149,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="23"/>
+      <c r="M18" s="22"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2167,10 +2170,10 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="23"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="22"/>
       <c r="G19" s="8" t="s">
         <v>136</v>
       </c>
@@ -2186,7 +2189,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="23"/>
+      <c r="M19" s="22"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2207,9 +2210,9 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
@@ -2225,7 +2228,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="23"/>
+      <c r="M20" s="22"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2249,9 +2252,9 @@
       </c>
     </row>
     <row r="21" spans="1:23" ht="75">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
       <c r="G21" s="20" t="s">
         <v>198</v>
       </c>
@@ -2267,7 +2270,7 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="23"/>
+      <c r="M21" s="22"/>
       <c r="N21" s="2" t="s">
         <v>195</v>
       </c>
@@ -2288,9 +2291,9 @@
       </c>
     </row>
     <row r="22" spans="1:23" ht="105">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
       <c r="G22" s="21" t="s">
         <v>182</v>
       </c>
@@ -2306,7 +2309,7 @@
       <c r="K22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="23"/>
+      <c r="M22" s="22"/>
       <c r="N22" s="2" t="s">
         <v>183</v>
       </c>
@@ -2324,14 +2327,14 @@
       </c>
     </row>
     <row r="23" spans="1:23" ht="90">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="23" t="s">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
       <c r="G23" s="2" t="s">
         <v>117</v>
       </c>
@@ -2347,7 +2350,7 @@
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="23"/>
+      <c r="M23" s="22"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2368,12 +2371,12 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="45">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="2" t="s">
         <v>116</v>
       </c>
@@ -2389,7 +2392,7 @@
       <c r="K24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="23"/>
+      <c r="M24" s="22"/>
       <c r="N24" s="2" t="s">
         <v>57</v>
       </c>
@@ -2413,14 +2416,14 @@
       </c>
     </row>
     <row r="25" spans="1:23" ht="90">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="23" t="s">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23" t="s">
+      <c r="E25" s="22"/>
+      <c r="F25" s="22" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2438,7 +2441,7 @@
       <c r="K25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="23" t="s">
+      <c r="M25" s="22" t="s">
         <v>108</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -2458,12 +2461,12 @@
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="2" t="s">
         <v>45</v>
       </c>
@@ -2476,7 +2479,7 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="23"/>
+      <c r="M26" s="22"/>
       <c r="S26" s="2">
         <v>-117.531786</v>
       </c>
@@ -2485,12 +2488,12 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
       <c r="G27" s="2" t="s">
         <v>46</v>
       </c>
@@ -2503,7 +2506,7 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="23"/>
+      <c r="M27" s="22"/>
       <c r="S27" s="2">
         <v>-110.655421</v>
       </c>
@@ -2512,12 +2515,12 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
       <c r="G28" s="2" t="s">
         <v>47</v>
       </c>
@@ -2530,7 +2533,7 @@
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="23"/>
+      <c r="M28" s="22"/>
       <c r="S28" s="2">
         <v>41.946097000000002</v>
       </c>
@@ -2539,12 +2542,12 @@
       </c>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
       <c r="G29" s="2" t="s">
         <v>48</v>
       </c>
@@ -2557,7 +2560,7 @@
       <c r="K29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M29" s="23"/>
+      <c r="M29" s="22"/>
       <c r="S29" s="2">
         <v>49.039541999999997</v>
       </c>
@@ -2566,12 +2569,12 @@
       </c>
     </row>
     <row r="30" spans="1:23" ht="30">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22" t="s">
         <v>51</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -2586,18 +2589,18 @@
       <c r="K30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="23"/>
+      <c r="M30" s="22"/>
       <c r="T30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
       <c r="G31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2610,18 +2613,18 @@
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="23"/>
+      <c r="M31" s="22"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:23">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
       <c r="G32" s="2" t="s">
         <v>54</v>
       </c>
@@ -2634,18 +2637,18 @@
       <c r="K32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M32" s="23"/>
+      <c r="M32" s="22"/>
       <c r="T32" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="30">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22" t="s">
         <v>191</v>
       </c>
       <c r="G33" s="2" t="s">
@@ -2660,18 +2663,18 @@
       <c r="K33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M33" s="23"/>
+      <c r="M33" s="22"/>
       <c r="T33" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="2" t="s">
         <v>192</v>
       </c>
@@ -2684,18 +2687,18 @@
       <c r="K34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="23"/>
+      <c r="M34" s="22"/>
       <c r="T34" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
       <c r="G35" s="2" t="s">
         <v>193</v>
       </c>
@@ -2708,23 +2711,23 @@
       <c r="K35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="23"/>
+      <c r="M35" s="22"/>
       <c r="T35" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="85" customHeight="1">
-      <c r="A36" s="24"/>
-      <c r="B36" s="23" t="s">
+      <c r="A36" s="23"/>
+      <c r="B36" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="24" t="s">
         <v>101</v>
       </c>
       <c r="F36" s="2"/>
@@ -2763,11 +2766,11 @@
       </c>
     </row>
     <row r="37" spans="1:23" ht="30" customHeight="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="2"/>
       <c r="G37" s="10" t="s">
         <v>124</v>
@@ -2781,7 +2784,7 @@
       <c r="K37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="23" t="s">
+      <c r="M37" s="22" t="s">
         <v>107</v>
       </c>
       <c r="N37" s="12" t="s">
@@ -2792,11 +2795,11 @@
       </c>
     </row>
     <row r="38" spans="1:23" ht="30">
-      <c r="A38" s="24"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="25"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="7"/>
       <c r="G38" s="2" t="s">
         <v>126</v>
@@ -2810,7 +2813,7 @@
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="23"/>
+      <c r="M38" s="22"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
@@ -2822,12 +2825,12 @@
       </c>
     </row>
     <row r="39" spans="1:23">
-      <c r="A39" s="24"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="23" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="2" t="s">
@@ -2839,7 +2842,7 @@
       <c r="K39" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M39" s="23"/>
+      <c r="M39" s="22"/>
       <c r="N39" s="2" t="s">
         <v>77</v>
       </c>
@@ -2851,12 +2854,12 @@
       </c>
     </row>
     <row r="40" spans="1:23" ht="30">
-      <c r="A40" s="24"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="23"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="22"/>
       <c r="G40" s="2" t="s">
         <v>16</v>
       </c>
@@ -2869,7 +2872,7 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="23"/>
+      <c r="M40" s="22"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
@@ -2881,12 +2884,12 @@
       </c>
     </row>
     <row r="41" spans="1:23" ht="30">
-      <c r="A41" s="24"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="23"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="22"/>
       <c r="G41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2899,7 +2902,7 @@
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="23"/>
+      <c r="M41" s="22"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
@@ -2911,12 +2914,12 @@
       </c>
     </row>
     <row r="42" spans="1:23" ht="30">
-      <c r="A42" s="24"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="23"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="22"/>
       <c r="G42" s="2" t="s">
         <v>19</v>
       </c>
@@ -2929,7 +2932,7 @@
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="23"/>
+      <c r="M42" s="22"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
@@ -2941,12 +2944,12 @@
       </c>
     </row>
     <row r="43" spans="1:23" ht="30">
-      <c r="A43" s="24"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="23"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="22"/>
       <c r="G43" s="2" t="s">
         <v>20</v>
       </c>
@@ -2959,7 +2962,7 @@
       <c r="K43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M43" s="23"/>
+      <c r="M43" s="22"/>
       <c r="N43" s="2" t="s">
         <v>57</v>
       </c>
@@ -2971,12 +2974,12 @@
       </c>
     </row>
     <row r="44" spans="1:23" ht="30">
-      <c r="A44" s="24"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="23"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="22"/>
       <c r="G44" s="2" t="s">
         <v>69</v>
       </c>
@@ -2989,7 +2992,7 @@
       <c r="K44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="23"/>
+      <c r="M44" s="22"/>
       <c r="N44" s="2" t="s">
         <v>57</v>
       </c>
@@ -3001,12 +3004,12 @@
       </c>
     </row>
     <row r="45" spans="1:23" ht="45">
-      <c r="A45" s="24"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="23"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="22"/>
       <c r="G45" s="2" t="s">
         <v>15</v>
       </c>
@@ -3019,7 +3022,7 @@
       <c r="K45" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M45" s="23"/>
+      <c r="M45" s="22"/>
       <c r="N45" s="2" t="s">
         <v>57</v>
       </c>
@@ -3034,12 +3037,12 @@
       </c>
     </row>
     <row r="46" spans="1:23" ht="30">
-      <c r="A46" s="24"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="23"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="22"/>
       <c r="G46" s="2" t="s">
         <v>21</v>
       </c>
@@ -3052,7 +3055,7 @@
       <c r="K46" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M46" s="23"/>
+      <c r="M46" s="22"/>
       <c r="N46" s="2" t="s">
         <v>57</v>
       </c>
@@ -3063,12 +3066,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="30">
-      <c r="A47" s="24"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
-      <c r="E47" s="25"/>
+    <row r="47" spans="1:23" ht="90">
+      <c r="A47" s="23"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="24"/>
       <c r="F47" s="19"/>
       <c r="G47" s="2" t="s">
         <v>201</v>
@@ -3095,16 +3098,19 @@
       <c r="T47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V47" s="26" t="s">
+      <c r="U47" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="V47" s="18" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="90">
-      <c r="A48" s="24"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="24"/>
       <c r="G48" s="18" t="s">
         <v>52</v>
       </c>
@@ -3140,7 +3146,7 @@
       </c>
     </row>
     <row r="49" spans="1:23" ht="30">
-      <c r="A49" s="24"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="3" t="s">
         <v>94</v>
       </c>
@@ -3183,7 +3189,7 @@
       </c>
     </row>
     <row r="50" spans="1:23" ht="30">
-      <c r="A50" s="24"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="3" t="s">
         <v>148</v>
       </c>
@@ -3484,6 +3490,18 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="D3:D15"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="E5:E15"/>
+    <mergeCell ref="D25:D35"/>
+    <mergeCell ref="C3:C35"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
     <mergeCell ref="M37:M46"/>
     <mergeCell ref="A3:A50"/>
     <mergeCell ref="B3:B35"/>
@@ -3499,18 +3517,6 @@
     <mergeCell ref="C36:C48"/>
     <mergeCell ref="B36:B48"/>
     <mergeCell ref="E36:E48"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="E25:E29"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D25:D35"/>
-    <mergeCell ref="C3:C35"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F30:F32"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
updates to the Excel design doc, delted vertical extents, added compression technique and format version, removed highlighting
</commit_message>
<xml_diff>
--- a/design_doc/MetadataEditor_DesignDoc.xlsx
+++ b/design_doc/MetadataEditor_DesignDoc.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="42240" yWindow="-2460" windowWidth="22320" windowHeight="18680" tabRatio="500"/>
+    <workbookView xWindow="29260" yWindow="-5120" windowWidth="20100" windowHeight="22180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$50</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$49</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$G:$G,Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="209">
   <si>
     <t>Required?</t>
   </si>
@@ -457,9 +457,6 @@
     <t>List keywords that will help others discover your data through an intuitive search. In addition to subject-based keywords, you may also want to include the grant numbers and funding sources associated with creation of the data.</t>
   </si>
   <si>
-    <t>What is the geographic area covered by the data? [For the MILES project, the defaults here are for the entire state of Idaho].</t>
-  </si>
-  <si>
     <t>Identify the organization and, where appropriate, the point of contact (name or position, e.g., Data Manager) responsible for providing physical access to the data. NKN's information is provided as a default.</t>
   </si>
   <si>
@@ -596,18 +593,6 @@
   </si>
   <si>
     <t>Needs to be editable; even if NKN is choosen as distributor</t>
-  </si>
-  <si>
-    <t>Vertical Extent</t>
-  </si>
-  <si>
-    <t>Vertical Minimum</t>
-  </si>
-  <si>
-    <t>Vertical Maximum</t>
-  </si>
-  <si>
-    <t>What is the minimum and maximum vertical heights covered by the data? (if applicable)</t>
   </si>
   <si>
     <t>&lt;gmd:MD_SpatialRepresentationTypeCode</t>
@@ -645,6 +630,27 @@
   <si>
     <t>Dropdown values plus Type In option
 Allow multiple selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the geographic area covered by the data? Please enter lat/lon as decimal degrees. </t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Compression Technique</t>
+  </si>
+  <si>
+    <t>on Data Format</t>
+  </si>
+  <si>
+    <t>Write-in (default should be N/A)</t>
+  </si>
+  <si>
+    <t>Is your data offered in a compressed format? If so please type a short description here. For example, "The LAS files are compressed in standard ZIP format."</t>
+  </si>
+  <si>
+    <t>Version</t>
   </si>
 </sst>
 </file>
@@ -697,18 +703,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -720,7 +720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -900,8 +900,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -921,12 +925,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -945,20 +943,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -969,17 +958,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1069,6 +1079,8 @@
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1158,6 +1170,8 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1490,13 +1504,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W57"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="T46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V47" sqref="V47"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1504,10 +1518,11 @@
     <col min="1" max="1" width="14.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="13" style="3" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="38.33203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="14" customWidth="1"/>
+    <col min="8" max="8" width="38.33203125" style="8" customWidth="1"/>
     <col min="9" max="9" width="26.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.1640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="12.5" style="2" customWidth="1"/>
@@ -1526,18 +1541,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="45">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="7" t="s">
         <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -1591,17 +1606,17 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="17" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>176</v>
-      </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1609,29 +1624,29 @@
         <v>7</v>
       </c>
       <c r="U2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="V2" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="V2" s="5" t="s">
-        <v>189</v>
-      </c>
     </row>
     <row r="3" spans="1:23" ht="74" customHeight="1">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="8" t="s">
         <v>119</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1643,7 +1658,7 @@
       <c r="K3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="19" t="s">
         <v>107</v>
       </c>
       <c r="N3" s="2" t="s">
@@ -1660,14 +1675,14 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="30">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="G4" s="8" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="G4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1679,7 +1694,7 @@
       <c r="K4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="22"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1697,20 +1712,20 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="75">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="F5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>125</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1722,7 +1737,7 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="22"/>
+      <c r="M5" s="19"/>
       <c r="O5" s="2" t="s">
         <v>86</v>
       </c>
@@ -1734,13 +1749,13 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="30">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="25"/>
+      <c r="G6" s="14" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1752,7 +1767,7 @@
       <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="22"/>
+      <c r="M6" s="19"/>
       <c r="N6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1767,13 +1782,13 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="30">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="24"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="14" t="s">
         <v>124</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1785,7 +1800,7 @@
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="22"/>
+      <c r="M7" s="19"/>
       <c r="N7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1794,15 +1809,15 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="45">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="14" t="s">
         <v>73</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1814,7 +1829,7 @@
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="22"/>
+      <c r="M8" s="19"/>
       <c r="N8" s="2" t="s">
         <v>77</v>
       </c>
@@ -1829,13 +1844,13 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="30">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="2" t="s">
+      <c r="F9" s="24"/>
+      <c r="G9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1847,7 +1862,7 @@
       <c r="K9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M9" s="22"/>
+      <c r="M9" s="19"/>
       <c r="N9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1862,13 +1877,13 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="30">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="24"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="14" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1880,7 +1895,7 @@
       <c r="K10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="22"/>
+      <c r="M10" s="19"/>
       <c r="N10" s="2" t="s">
         <v>57</v>
       </c>
@@ -1892,13 +1907,13 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="30">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="24"/>
+      <c r="G11" s="14" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1910,7 +1925,7 @@
       <c r="K11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M11" s="22"/>
+      <c r="M11" s="19"/>
       <c r="N11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1928,13 +1943,13 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="30">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="24"/>
+      <c r="G12" s="14" t="s">
         <v>20</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -1946,7 +1961,7 @@
       <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M12" s="22"/>
+      <c r="M12" s="19"/>
       <c r="N12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1958,13 +1973,13 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="30">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="14" t="s">
         <v>69</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -1976,7 +1991,7 @@
       <c r="K13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M13" s="22"/>
+      <c r="M13" s="19"/>
       <c r="N13" s="2" t="s">
         <v>57</v>
       </c>
@@ -1994,13 +2009,13 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="45">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="24"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="14" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -2012,7 +2027,7 @@
       <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="22"/>
+      <c r="M14" s="19"/>
       <c r="N14" s="2" t="s">
         <v>57</v>
       </c>
@@ -2027,13 +2042,13 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="30">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="24"/>
+      <c r="G15" s="14" t="s">
         <v>21</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -2045,7 +2060,7 @@
       <c r="K15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M15" s="22"/>
+      <c r="M15" s="19"/>
       <c r="N15" s="2" t="s">
         <v>57</v>
       </c>
@@ -2057,16 +2072,16 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="105">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="8" t="s">
         <v>122</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -2078,7 +2093,7 @@
       <c r="K16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="19" t="s">
         <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
@@ -2092,13 +2107,13 @@
       </c>
     </row>
     <row r="17" spans="1:23" ht="120">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="14" t="s">
         <v>30</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -2113,7 +2128,7 @@
       <c r="K17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="22"/>
+      <c r="M17" s="19"/>
       <c r="N17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2128,16 +2143,16 @@
       </c>
     </row>
     <row r="18" spans="1:23" ht="90">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="8" t="s">
         <v>143</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -2149,7 +2164,7 @@
       <c r="K18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="22"/>
+      <c r="M18" s="19"/>
       <c r="N18" s="2" t="s">
         <v>57</v>
       </c>
@@ -2170,14 +2185,14 @@
       </c>
     </row>
     <row r="19" spans="1:23" ht="90">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="22"/>
-      <c r="G19" s="8" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
+      <c r="G19" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="8" t="s">
         <v>137</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -2189,7 +2204,7 @@
       <c r="K19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="22"/>
+      <c r="M19" s="19"/>
       <c r="N19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2200,7 +2215,7 @@
         <v>98</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T19" s="2" t="s">
         <v>6</v>
@@ -2210,14 +2225,14 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="90">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
       <c r="G20" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="H20" s="10" t="s">
-        <v>181</v>
+      <c r="H20" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>38</v>
@@ -2228,7 +2243,7 @@
       <c r="K20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="22"/>
+      <c r="M20" s="19"/>
       <c r="N20" s="2" t="s">
         <v>141</v>
       </c>
@@ -2248,18 +2263,18 @@
         <v>140</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="75">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="G21" s="20" t="s">
-        <v>198</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>200</v>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="G21" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>38</v>
@@ -2270,12 +2285,12 @@
       <c r="K21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M21" s="22"/>
+      <c r="M21" s="19"/>
       <c r="N21" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Q21" s="2" t="s">
         <v>139</v>
@@ -2284,21 +2299,21 @@
         <v>7</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="105">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="G22" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="H22" s="10" t="s">
-        <v>185</v>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="G22" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>184</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>38</v>
@@ -2309,33 +2324,33 @@
       <c r="K22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M22" s="22"/>
+      <c r="M22" s="19"/>
       <c r="N22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U22" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="O22" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="V22" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:23" ht="90">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="22" t="s">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="2" t="s">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="14" t="s">
         <v>117</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -2350,7 +2365,7 @@
       <c r="K23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M23" s="22"/>
+      <c r="M23" s="19"/>
       <c r="N23" s="2" t="s">
         <v>57</v>
       </c>
@@ -2371,13 +2386,13 @@
       </c>
     </row>
     <row r="24" spans="1:23" ht="45">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="2" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="14" t="s">
         <v>116</v>
       </c>
       <c r="H24" s="2" t="s">
@@ -2392,7 +2407,7 @@
       <c r="K24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="22"/>
+      <c r="M24" s="19"/>
       <c r="N24" s="2" t="s">
         <v>57</v>
       </c>
@@ -2416,21 +2431,21 @@
       </c>
     </row>
     <row r="25" spans="1:23" ht="90">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="22" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="24"/>
+      <c r="F25" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="14" t="s">
         <v>11</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>144</v>
+        <v>202</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>44</v>
@@ -2441,7 +2456,7 @@
       <c r="K25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="M25" s="19" t="s">
         <v>108</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -2461,13 +2476,13 @@
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="2" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="14" t="s">
         <v>45</v>
       </c>
       <c r="I26" s="2" t="s">
@@ -2479,7 +2494,7 @@
       <c r="K26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="22"/>
+      <c r="M26" s="19"/>
       <c r="S26" s="2">
         <v>-117.531786</v>
       </c>
@@ -2488,13 +2503,13 @@
       </c>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="2" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="14" t="s">
         <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
@@ -2506,7 +2521,7 @@
       <c r="K27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M27" s="22"/>
+      <c r="M27" s="19"/>
       <c r="S27" s="2">
         <v>-110.655421</v>
       </c>
@@ -2515,13 +2530,13 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="2" t="s">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="14" t="s">
         <v>47</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -2533,7 +2548,7 @@
       <c r="K28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M28" s="22"/>
+      <c r="M28" s="19"/>
       <c r="S28" s="2">
         <v>41.946097000000002</v>
       </c>
@@ -2542,13 +2557,13 @@
       </c>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="2" t="s">
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="14" t="s">
         <v>48</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -2560,7 +2575,7 @@
       <c r="K29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M29" s="22"/>
+      <c r="M29" s="19"/>
       <c r="S29" s="2">
         <v>49.039541999999997</v>
       </c>
@@ -2569,18 +2584,18 @@
       </c>
     </row>
     <row r="30" spans="1:23" ht="30">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22" t="s">
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="10" t="s">
+      <c r="G30" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>120</v>
       </c>
       <c r="J30" s="2" t="s">
@@ -2589,19 +2604,19 @@
       <c r="K30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M30" s="22"/>
+      <c r="M30" s="19"/>
       <c r="T30" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="2" t="s">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="14" t="s">
         <v>53</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -2613,19 +2628,19 @@
       <c r="K31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="22"/>
+      <c r="M31" s="19"/>
       <c r="T31" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:23">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="2" t="s">
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="14" t="s">
         <v>54</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -2637,25 +2652,34 @@
       <c r="K32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M32" s="22"/>
+      <c r="M32" s="19"/>
       <c r="T32" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="30">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>194</v>
+    <row r="33" spans="1:23" ht="85" customHeight="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33" s="14"/>
+      <c r="G33" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>11</v>
@@ -2663,82 +2687,95 @@
       <c r="K33" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M33" s="22"/>
+      <c r="L33" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="T33" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>41</v>
+        <v>127</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="30" customHeight="1">
+      <c r="A34" s="20"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="T34" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="2" t="s">
-        <v>193</v>
+    <row r="35" spans="1:23" ht="30">
+      <c r="A35" s="20"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M35" s="22"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="T35" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="85" customHeight="1">
-      <c r="A36" s="23"/>
-      <c r="B36" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>11</v>
+    <row r="36" spans="1:23">
+      <c r="A36" s="20"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>11</v>
@@ -2746,36 +2783,28 @@
       <c r="K36" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>172</v>
+      <c r="M36" s="19"/>
+      <c r="N36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="T36" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="W36" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" ht="30" customHeight="1">
-      <c r="A37" s="23"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="30">
+      <c r="A37" s="20"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
       <c r="E37" s="24"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I37" s="10" t="s">
+      <c r="F37" s="24"/>
+      <c r="G37" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>37</v>
       </c>
       <c r="J37" s="2" t="s">
@@ -2784,25 +2813,26 @@
       <c r="K37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M37" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="N37" s="12" t="s">
+      <c r="M37" s="19"/>
+      <c r="N37" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="O37" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="T37" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="30">
-      <c r="A38" s="23"/>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
       <c r="E38" s="24"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="2" t="s">
-        <v>126</v>
+      <c r="F38" s="24"/>
+      <c r="G38" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>37</v>
@@ -2813,58 +2843,59 @@
       <c r="K38" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="22"/>
+      <c r="M38" s="19"/>
       <c r="N38" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="T38" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
-      <c r="A39" s="23"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
+    <row r="39" spans="1:23" ht="30">
+      <c r="A39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>73</v>
+      <c r="F39" s="24"/>
+      <c r="G39" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M39" s="22"/>
+        <v>7</v>
+      </c>
+      <c r="M39" s="19"/>
       <c r="N39" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="T39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:23" ht="30">
-      <c r="A40" s="23"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="24"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="2" t="s">
-        <v>16</v>
+      <c r="F40" s="24"/>
+      <c r="G40" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>6</v>
@@ -2872,26 +2903,26 @@
       <c r="K40" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M40" s="22"/>
+      <c r="M40" s="19"/>
       <c r="N40" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="T40" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="30">
-      <c r="A41" s="23"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="24"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="2" t="s">
-        <v>18</v>
+      <c r="F41" s="24"/>
+      <c r="G41" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>37</v>
@@ -2902,59 +2933,62 @@
       <c r="K41" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M41" s="22"/>
+      <c r="M41" s="19"/>
       <c r="N41" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="T41" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="30">
-      <c r="A42" s="23"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
+    <row r="42" spans="1:23" ht="45">
+      <c r="A42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="24"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="2" t="s">
-        <v>19</v>
+      <c r="F42" s="24"/>
+      <c r="G42" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M42" s="22"/>
+      <c r="M42" s="19"/>
       <c r="N42" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="T42" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="30">
-      <c r="A43" s="23"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="24"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="2" t="s">
-        <v>20</v>
+      <c r="F43" s="24"/>
+      <c r="G43" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>6</v>
@@ -2962,29 +2996,34 @@
       <c r="K43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M43" s="22"/>
+      <c r="M43" s="19"/>
       <c r="N43" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="T43" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="30">
-      <c r="A44" s="23"/>
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
+    <row r="44" spans="1:23" ht="90">
+      <c r="A44" s="20"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="24"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="2" t="s">
-        <v>69</v>
+      <c r="F44" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>37</v>
+        <v>199</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>6</v>
@@ -2992,374 +3031,364 @@
       <c r="K44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M44" s="22"/>
+      <c r="M44" s="17"/>
       <c r="N44" s="2" t="s">
         <v>57</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>70</v>
+        <v>198</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" ht="45">
-      <c r="A45" s="23"/>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="22"/>
+        <v>6</v>
+      </c>
+      <c r="U44" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="V44" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
+      <c r="A45" s="20"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="24"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M45" s="22"/>
-      <c r="N45" s="2" t="s">
+      <c r="F45" s="24"/>
+      <c r="G45" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="M45" s="17"/>
+      <c r="V45" s="14"/>
+    </row>
+    <row r="46" spans="1:23" ht="60">
+      <c r="A46" s="20"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="M46" s="17"/>
+      <c r="V46" s="14"/>
+    </row>
+    <row r="47" spans="1:23" ht="90">
+      <c r="A47" s="20"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="24"/>
+      <c r="G47" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P47" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="T47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U47" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="30">
+      <c r="A48" s="20"/>
+      <c r="B48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U48" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="30">
+      <c r="A49" s="20"/>
+      <c r="B49" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="N49" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O45" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="T45" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" ht="30">
-      <c r="A46" s="23"/>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I46" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M46" s="22"/>
-      <c r="N46" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="T46" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" ht="90">
-      <c r="A47" s="23"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="H47" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M47" s="19"/>
-      <c r="N47" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O47" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="T47" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="U47" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="V47" s="18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" ht="90">
-      <c r="A48" s="23"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="24"/>
-      <c r="G48" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M48" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="P48" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="T48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="U48" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" ht="30">
-      <c r="A49" s="23"/>
-      <c r="B49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E49" s="15"/>
-      <c r="G49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M49" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="O49" s="2" t="s">
-        <v>95</v>
+        <v>151</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R49" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="T49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" ht="30">
-      <c r="A50" s="23"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23">
       <c r="B50" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" s="15"/>
-      <c r="G50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H50" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="J50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M50" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J50" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K50" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M50" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="N50" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="O50" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="R50" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="T50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U50" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:23">
       <c r="B51" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H51" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M51" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K51" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M51" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="O51" s="2" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R51" s="2" t="s">
-        <v>156</v>
+        <v>28</v>
       </c>
       <c r="T51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U51" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:23">
       <c r="B52" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M52" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J52" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K52" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M52" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="O52" s="2" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R52" s="2" t="s">
-        <v>28</v>
+        <v>159</v>
       </c>
       <c r="T52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U52" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="45">
+      <c r="B53" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="1:23">
-      <c r="B53" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H53" s="14" t="s">
+      <c r="G53" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>151</v>
+      <c r="N53" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R53" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="T53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U53" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="T53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U53" s="2" t="s">
-        <v>161</v>
+      <c r="W53" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:23" ht="45">
       <c r="B54" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="G54" s="3" t="s">
+      <c r="G54" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M54" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M54" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="N54" s="2" t="s">
         <v>57</v>
@@ -3373,81 +3402,66 @@
       <c r="Q54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="R54" s="2" t="s">
+      <c r="R54" s="2">
+        <v>2003</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="W54" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="T54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U54" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W54" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" ht="45">
+    </row>
+    <row r="55" spans="1:23">
       <c r="B55" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="H55" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="J55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K55" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M55" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="N55" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O55" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="P55" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q55" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="R55" s="2">
-        <v>2003</v>
+      <c r="R55" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="T55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U55" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="W55" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="75">
       <c r="B56" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G56" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M56" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K56" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M56" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="R56" s="2" t="s">
         <v>173</v>
@@ -3456,75 +3470,44 @@
         <v>7</v>
       </c>
       <c r="U56" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" ht="75">
-      <c r="B57" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M57" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="R57" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="T57" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U57" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="E25:E29"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="D3:D15"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="F8:F15"/>
-    <mergeCell ref="E5:E15"/>
-    <mergeCell ref="D25:D35"/>
-    <mergeCell ref="C3:C35"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="M37:M46"/>
-    <mergeCell ref="A3:A50"/>
-    <mergeCell ref="B3:B35"/>
+  <mergeCells count="26">
+    <mergeCell ref="M34:M43"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="B3:B32"/>
     <mergeCell ref="M3:M15"/>
-    <mergeCell ref="M25:M35"/>
+    <mergeCell ref="M25:M32"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="M16:M24"/>
-    <mergeCell ref="D36:D48"/>
-    <mergeCell ref="F39:F46"/>
-    <mergeCell ref="C36:C48"/>
-    <mergeCell ref="B36:B48"/>
-    <mergeCell ref="E36:E48"/>
+    <mergeCell ref="D33:D47"/>
+    <mergeCell ref="F36:F43"/>
+    <mergeCell ref="C33:C47"/>
+    <mergeCell ref="B33:B47"/>
+    <mergeCell ref="E33:E47"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="D3:D15"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="F8:F15"/>
+    <mergeCell ref="E5:E15"/>
+    <mergeCell ref="D25:D32"/>
+    <mergeCell ref="C3:C32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" headings="1" gridLines="1"/>
   <pageMargins left="0.75" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup scale="21" fitToHeight="2" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <rowBreaks count="2" manualBreakCount="2">
-    <brk id="32" max="16383" man="1"/>
-    <brk id="49" max="16383" man="1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="48" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>

</xml_diff>